<commit_message>
finish grouping for Mesos Master configuration
</commit_message>
<xml_diff>
--- a/configuration flags.xlsx
+++ b/configuration flags.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="110" windowWidth="14810" windowHeight="8010" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="110" windowWidth="14810" windowHeight="8010" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="master-flag" sheetId="1" r:id="rId1"/>
@@ -125,7 +125,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="344" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="151">
   <si>
     <t>Flag</t>
   </si>
@@ -1892,6 +1892,9 @@
   </si>
   <si>
     <t>metrics</t>
+  </si>
+  <si>
+    <t>allocation</t>
   </si>
 </sst>
 </file>
@@ -3149,8 +3152,8 @@
   </sheetPr>
   <dimension ref="A1:C43"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3425,7 +3428,9 @@
       <c r="B25" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="C25" s="19"/>
+      <c r="C25" s="19" t="s">
+        <v>144</v>
+      </c>
     </row>
     <row r="26" spans="1:3" ht="20.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A26" s="14" t="s">
@@ -3434,7 +3439,9 @@
       <c r="B26" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="C26" s="19"/>
+      <c r="C26" s="19" t="s">
+        <v>142</v>
+      </c>
     </row>
     <row r="27" spans="1:3" ht="30.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A27" s="14" t="s">
@@ -3443,7 +3450,9 @@
       <c r="B27" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="C27" s="19"/>
+      <c r="C27" s="19" t="s">
+        <v>144</v>
+      </c>
     </row>
     <row r="28" spans="1:3" ht="17.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A28" s="14" t="s">
@@ -3452,7 +3461,9 @@
       <c r="B28" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="C28" s="19"/>
+      <c r="C28" s="19" t="s">
+        <v>150</v>
+      </c>
     </row>
     <row r="29" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A29" s="14" t="s">
@@ -3461,7 +3472,9 @@
       <c r="B29" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="C29" s="19"/>
+      <c r="C29" s="19" t="s">
+        <v>144</v>
+      </c>
     </row>
     <row r="30" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A30" s="14" t="s">
@@ -3470,7 +3483,9 @@
       <c r="B30" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="C30" s="19"/>
+      <c r="C30" s="19" t="s">
+        <v>144</v>
+      </c>
     </row>
     <row r="31" spans="1:3" ht="70.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A31" s="14" t="s">
@@ -3479,7 +3494,9 @@
       <c r="B31" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="C31" s="19"/>
+      <c r="C31" s="19" t="s">
+        <v>150</v>
+      </c>
     </row>
     <row r="32" spans="1:3" ht="20.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A32" s="14" t="s">
@@ -3600,7 +3617,7 @@
   </sheetPr>
   <dimension ref="A1:C50"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
finish one version of Mesos agent flags
</commit_message>
<xml_diff>
--- a/configuration flags.xlsx
+++ b/configuration flags.xlsx
@@ -125,7 +125,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="378" uniqueCount="153">
   <si>
     <t>Flag</t>
   </si>
@@ -1946,7 +1946,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2019,6 +2019,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -2065,7 +2071,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1" indent="1"/>
@@ -2144,6 +2150,18 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -3204,7 +3222,7 @@
   <dimension ref="A1:C43"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3669,7 +3687,7 @@
   <dimension ref="A1:C50"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="B6" sqref="B6:B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3757,7 +3775,9 @@
       <c r="B8" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="C8" s="16"/>
+      <c r="C8" s="27" t="s">
+        <v>143</v>
+      </c>
     </row>
     <row r="9" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A9" s="14" t="s">
@@ -3775,7 +3795,9 @@
       <c r="B10" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="C10" s="16"/>
+      <c r="C10" s="16" t="s">
+        <v>143</v>
+      </c>
     </row>
     <row r="11" spans="1:3" ht="20.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A11" s="14" t="s">
@@ -3784,7 +3806,9 @@
       <c r="B11" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="C11" s="16"/>
+      <c r="C11" s="16" t="s">
+        <v>143</v>
+      </c>
     </row>
     <row r="12" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A12" s="14" t="s">
@@ -3793,7 +3817,9 @@
       <c r="B12" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="C12" s="16"/>
+      <c r="C12" s="16" t="s">
+        <v>143</v>
+      </c>
     </row>
     <row r="13" spans="1:3" ht="20.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A13" s="14" t="s">
@@ -3802,7 +3828,9 @@
       <c r="B13" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="C13" s="16"/>
+      <c r="C13" s="16" t="s">
+        <v>143</v>
+      </c>
     </row>
     <row r="14" spans="1:3" ht="20.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A14" s="14" t="s">
@@ -3811,7 +3839,9 @@
       <c r="B14" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="C14" s="16"/>
+      <c r="C14" s="16" t="s">
+        <v>143</v>
+      </c>
     </row>
     <row r="15" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A15" s="14" t="s">
@@ -3820,7 +3850,9 @@
       <c r="B15" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="C15" s="16"/>
+      <c r="C15" s="16" t="s">
+        <v>144</v>
+      </c>
     </row>
     <row r="16" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A16" s="14" t="s">
@@ -3829,7 +3861,9 @@
       <c r="B16" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C16" s="16"/>
+      <c r="C16" s="27" t="s">
+        <v>144</v>
+      </c>
     </row>
     <row r="17" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A17" s="14" t="s">
@@ -3838,7 +3872,9 @@
       <c r="B17" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C17" s="16"/>
+      <c r="C17" s="16" t="s">
+        <v>144</v>
+      </c>
     </row>
     <row r="18" spans="1:3" ht="30.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A18" s="14" t="s">
@@ -3847,7 +3883,9 @@
       <c r="B18" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="C18" s="16"/>
+      <c r="C18" s="16" t="s">
+        <v>144</v>
+      </c>
     </row>
     <row r="19" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A19" s="14" t="s">
@@ -3856,7 +3894,9 @@
       <c r="B19" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="C19" s="16"/>
+      <c r="C19" s="16" t="s">
+        <v>144</v>
+      </c>
     </row>
     <row r="20" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A20" s="14" t="s">
@@ -3865,7 +3905,9 @@
       <c r="B20" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C20" s="16"/>
+      <c r="C20" s="16" t="s">
+        <v>145</v>
+      </c>
     </row>
     <row r="21" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A21" s="14" t="s">
@@ -3874,7 +3916,9 @@
       <c r="B21" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C21" s="16"/>
+      <c r="C21" s="16" t="s">
+        <v>145</v>
+      </c>
     </row>
     <row r="22" spans="1:3" ht="17.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A22" s="14" t="s">
@@ -3883,112 +3927,116 @@
       <c r="B22" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="C22" s="16"/>
-    </row>
-    <row r="23" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C22" s="16" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23" s="17" t="s">
         <v>108</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="C23" s="16"/>
-    </row>
-    <row r="24" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C23" s="28" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A24" s="19"/>
       <c r="B24" s="5" t="s">
         <v>110</v>
       </c>
-      <c r="C24" s="16"/>
-    </row>
-    <row r="25" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C24" s="29"/>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A25" s="19"/>
       <c r="B25" s="5" t="s">
         <v>111</v>
       </c>
-      <c r="C25" s="16"/>
-    </row>
-    <row r="26" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C25" s="29"/>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A26" s="19"/>
       <c r="B26" s="5" t="s">
         <v>112</v>
       </c>
-      <c r="C26" s="16"/>
-    </row>
-    <row r="27" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C26" s="29"/>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A27" s="19"/>
       <c r="B27" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="C27" s="16"/>
-    </row>
-    <row r="28" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C27" s="29"/>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A28" s="19"/>
       <c r="B28" s="3"/>
-      <c r="C28" s="16"/>
-    </row>
-    <row r="29" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C28" s="29"/>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A29" s="19"/>
       <c r="B29" s="11" t="s">
         <v>114</v>
       </c>
-      <c r="C29" s="16"/>
-    </row>
-    <row r="30" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C29" s="29"/>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A30" s="19"/>
       <c r="B30" s="12" t="s">
         <v>115</v>
       </c>
-      <c r="C30" s="16"/>
-    </row>
-    <row r="31" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C30" s="29"/>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A31" s="19"/>
       <c r="B31" s="6" t="s">
         <v>116</v>
       </c>
-      <c r="C31" s="16"/>
-    </row>
-    <row r="32" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C31" s="29"/>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A32" s="19"/>
       <c r="B32" s="6" t="s">
         <v>117</v>
       </c>
-      <c r="C32" s="16"/>
-    </row>
-    <row r="33" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C32" s="29"/>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A33" s="19"/>
       <c r="B33" s="12" t="s">
         <v>118</v>
       </c>
-      <c r="C33" s="16"/>
-    </row>
-    <row r="34" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C33" s="29"/>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A34" s="19"/>
       <c r="B34" s="6" t="s">
         <v>119</v>
       </c>
-      <c r="C34" s="16"/>
-    </row>
-    <row r="35" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C34" s="29"/>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A35" s="19"/>
       <c r="B35" s="6" t="s">
         <v>120</v>
       </c>
-      <c r="C35" s="16"/>
-    </row>
-    <row r="36" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C35" s="29"/>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A36" s="19"/>
       <c r="B36" s="12" t="s">
         <v>121</v>
       </c>
-      <c r="C36" s="16"/>
+      <c r="C36" s="29"/>
     </row>
     <row r="37" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A37" s="18"/>
       <c r="B37" s="6" t="s">
         <v>122</v>
       </c>
-      <c r="C37" s="16"/>
+      <c r="C37" s="30"/>
     </row>
     <row r="38" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A38" s="14" t="s">
@@ -3997,7 +4045,9 @@
       <c r="B38" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="C38" s="16"/>
+      <c r="C38" s="16" t="s">
+        <v>144</v>
+      </c>
     </row>
     <row r="39" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A39" s="14" t="s">
@@ -4006,7 +4056,9 @@
       <c r="B39" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="C39" s="16"/>
+      <c r="C39" s="16" t="s">
+        <v>145</v>
+      </c>
     </row>
     <row r="40" spans="1:3" ht="40.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A40" s="14" t="s">
@@ -4015,7 +4067,9 @@
       <c r="B40" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="C40" s="16"/>
+      <c r="C40" s="16" t="s">
+        <v>125</v>
+      </c>
     </row>
     <row r="41" spans="1:3" ht="30.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A41" s="14" t="s">
@@ -4024,7 +4078,9 @@
       <c r="B41" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="C41" s="16"/>
+      <c r="C41" s="16" t="s">
+        <v>125</v>
+      </c>
     </row>
     <row r="42" spans="1:3" ht="30.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A42" s="14" t="s">
@@ -4042,31 +4098,35 @@
       <c r="B43" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="C43" s="16"/>
-    </row>
-    <row r="44" spans="1:3" ht="27.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C43" s="16" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" ht="27" x14ac:dyDescent="0.35">
       <c r="A44" s="17" t="s">
         <v>132</v>
       </c>
       <c r="B44" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="C44" s="16"/>
-    </row>
-    <row r="45" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C44" s="28" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A45" s="19"/>
       <c r="B45" s="6" t="e">
         <f>--resources="cpus(prod):8; cpus(stage):2 mem(*):15360; disk(*):710534; ports(*):[31000-32000]"</f>
         <v>#VALUE!</v>
       </c>
-      <c r="C45" s="16"/>
+      <c r="C45" s="29"/>
     </row>
     <row r="46" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A46" s="18"/>
       <c r="B46" s="4" t="s">
         <v>134</v>
       </c>
-      <c r="C46" s="16"/>
+      <c r="C46" s="30"/>
     </row>
     <row r="47" spans="1:3" ht="30.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A47" s="14" t="s">
@@ -4075,7 +4135,9 @@
       <c r="B47" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="C47" s="16"/>
+      <c r="C47" s="16" t="s">
+        <v>125</v>
+      </c>
     </row>
     <row r="48" spans="1:3" ht="20.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A48" s="14" t="s">
@@ -4084,7 +4146,9 @@
       <c r="B48" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="C48" s="16"/>
+      <c r="C48" s="16" t="s">
+        <v>144</v>
+      </c>
     </row>
     <row r="49" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A49" s="14" t="s">
@@ -4093,7 +4157,9 @@
       <c r="B49" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="C49" s="16"/>
+      <c r="C49" s="16" t="s">
+        <v>144</v>
+      </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A50" s="14" t="s">
@@ -4102,20 +4168,25 @@
       <c r="B50" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="C50" s="16"/>
+      <c r="C50" s="16" t="s">
+        <v>144</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="7">
     <mergeCell ref="A6:A7"/>
     <mergeCell ref="A23:A37"/>
     <mergeCell ref="A44:A46"/>
     <mergeCell ref="C6:C7"/>
     <mergeCell ref="B6:B7"/>
+    <mergeCell ref="C23:C37"/>
+    <mergeCell ref="C44:C46"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B4" r:id="rId1" location="containerizer" display="https://open.mesosphere.com/reference/glossary/ - containerizer"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="0" r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
add UI fields for Mesos agent
</commit_message>
<xml_diff>
--- a/configuration flags.xlsx
+++ b/configuration flags.xlsx
@@ -1,21 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="27022"/>
-  <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+  <workbookPr filterPrivacy="1" autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="120" windowWidth="14820" windowHeight="8020" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12840" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="master-flag" sheetId="1" r:id="rId1"/>
     <sheet name="agent-flag" sheetId="2" r:id="rId2"/>
     <sheet name="master-flag-group" sheetId="4" r:id="rId3"/>
     <sheet name="agent-flag-group" sheetId="5" r:id="rId4"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId5"/>
+    <sheet name="fileds" sheetId="3" r:id="rId5"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId6"/>
-  </externalReferences>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'master-flag-group'!$A$1:$D$43</definedName>
     <definedName name="allocation_interval" localSheetId="0">'master-flag'!$A$2</definedName>
@@ -123,7 +120,7 @@
     <definedName name="zk_session_timeout" localSheetId="0">'master-flag'!$A$43</definedName>
     <definedName name="zk_session_timeout" localSheetId="2">'master-flag-group'!$A$43</definedName>
   </definedNames>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="152511" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -133,7 +130,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="446" uniqueCount="186">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="480" uniqueCount="192">
   <si>
     <t>Flag</t>
   </si>
@@ -2047,6 +2044,24 @@
   </si>
   <si>
     <t>INFO</t>
+  </si>
+  <si>
+    <t>1 mins</t>
+  </si>
+  <si>
+    <t>1 weeks</t>
+  </si>
+  <si>
+    <t>--no_version</t>
+  </si>
+  <si>
+    <t>radio Buttons</t>
+  </si>
+  <si>
+    <t>--switch_user</t>
+  </si>
+  <si>
+    <t>--strict</t>
   </si>
 </sst>
 </file>
@@ -2056,7 +2071,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="00000"/>
   </numFmts>
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2143,6 +2158,18 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -2198,7 +2225,7 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1" indent="1"/>
@@ -2266,6 +2293,8 @@
     <xf numFmtId="0" fontId="11" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -2305,8 +2334,17 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="11">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -2332,27 +2370,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="master-flag"/>
-      <sheetName val="agent-flag"/>
-      <sheetName val="master-flag-group"/>
-      <sheetName val="agent-flag-group"/>
-      <sheetName val="Sheet3"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0" refreshError="1"/>
-      <sheetData sheetId="1" refreshError="1"/>
-      <sheetData sheetId="2" refreshError="1"/>
-      <sheetData sheetId="3" refreshError="1"/>
-      <sheetData sheetId="4"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2642,7 +2659,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr enableFormatConditionsCalculation="0">
+  <sheetPr>
     <tabColor theme="5" tint="0.39997558519241921"/>
   </sheetPr>
   <dimension ref="A1:B43"/>
@@ -2651,13 +2668,13 @@
       <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="14.5" style="15" customWidth="1"/>
-    <col min="2" max="2" width="82.33203125" customWidth="1"/>
+    <col min="1" max="1" width="14.453125" style="15" customWidth="1"/>
+    <col min="2" max="2" width="82.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15" thickBot="1">
+    <row r="1" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
@@ -2665,7 +2682,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="15" thickBot="1">
+    <row r="2" spans="1:2" ht="17.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="14" t="s">
         <v>2</v>
       </c>
@@ -2673,7 +2690,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="31" thickBot="1">
+    <row r="3" spans="1:2" ht="30.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="14" t="s">
         <v>4</v>
       </c>
@@ -2681,7 +2698,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="31" thickBot="1">
+    <row r="4" spans="1:2" ht="40.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A4" s="14" t="s">
         <v>6</v>
       </c>
@@ -2689,7 +2706,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="15" thickBot="1">
+    <row r="5" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" s="14" t="s">
         <v>8</v>
       </c>
@@ -2697,7 +2714,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="41" thickBot="1">
+    <row r="6" spans="1:2" ht="40.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A6" s="14" t="s">
         <v>10</v>
       </c>
@@ -2705,7 +2722,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="19" thickBot="1">
+    <row r="7" spans="1:2" ht="20.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A7" s="14" t="s">
         <v>12</v>
       </c>
@@ -2713,7 +2730,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="15" thickBot="1">
+    <row r="8" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A8" s="14" t="s">
         <v>14</v>
       </c>
@@ -2721,7 +2738,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="15" thickBot="1">
+    <row r="9" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A9" s="14" t="s">
         <v>16</v>
       </c>
@@ -2729,7 +2746,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="15" thickBot="1">
+    <row r="10" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A10" s="14" t="s">
         <v>18</v>
       </c>
@@ -2737,7 +2754,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="31" thickBot="1">
+    <row r="11" spans="1:2" ht="30.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A11" s="14" t="s">
         <v>20</v>
       </c>
@@ -2745,7 +2762,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="15" thickBot="1">
+    <row r="12" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A12" s="14" t="s">
         <v>22</v>
       </c>
@@ -2753,7 +2770,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="15" thickBot="1">
+    <row r="13" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A13" s="14" t="s">
         <v>24</v>
       </c>
@@ -2761,7 +2778,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="15" thickBot="1">
+    <row r="14" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A14" s="14" t="s">
         <v>26</v>
       </c>
@@ -2769,7 +2786,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="15" spans="1:2" ht="15" thickBot="1">
+    <row r="15" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A15" s="14" t="s">
         <v>28</v>
       </c>
@@ -2777,7 +2794,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="16" spans="1:2" ht="15" thickBot="1">
+    <row r="16" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A16" s="14" t="s">
         <v>30</v>
       </c>
@@ -2785,21 +2802,21 @@
         <v>31</v>
       </c>
     </row>
-    <row r="17" spans="1:2" ht="20">
-      <c r="A17" s="23" t="s">
+    <row r="17" spans="1:2" ht="20" x14ac:dyDescent="0.35">
+      <c r="A17" s="25" t="s">
         <v>32</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="18" spans="1:2" ht="15" thickBot="1">
-      <c r="A18" s="24"/>
+    <row r="18" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A18" s="26"/>
       <c r="B18" s="4" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="19" spans="1:2" ht="51" thickBot="1">
+    <row r="19" spans="1:2" ht="60.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A19" s="14" t="s">
         <v>35</v>
       </c>
@@ -2807,7 +2824,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="20" spans="1:2" ht="19" thickBot="1">
+    <row r="20" spans="1:2" ht="17.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A20" s="14" t="s">
         <v>37</v>
       </c>
@@ -2815,7 +2832,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="21" spans="1:2" ht="19" thickBot="1">
+    <row r="21" spans="1:2" ht="20.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A21" s="14" t="s">
         <v>39</v>
       </c>
@@ -2823,7 +2840,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="22" spans="1:2" ht="21" thickBot="1">
+    <row r="22" spans="1:2" ht="20.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A22" s="14" t="s">
         <v>41</v>
       </c>
@@ -2831,7 +2848,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="23" spans="1:2" ht="19" thickBot="1">
+    <row r="23" spans="1:2" ht="20.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A23" s="14" t="s">
         <v>43</v>
       </c>
@@ -2839,7 +2856,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="24" spans="1:2" ht="31" thickBot="1">
+    <row r="24" spans="1:2" ht="30.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A24" s="14" t="s">
         <v>45</v>
       </c>
@@ -2847,7 +2864,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="25" spans="1:2" ht="15" thickBot="1">
+    <row r="25" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A25" s="14" t="s">
         <v>47</v>
       </c>
@@ -2855,7 +2872,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="26" spans="1:2" ht="21" thickBot="1">
+    <row r="26" spans="1:2" ht="20.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A26" s="14" t="s">
         <v>49</v>
       </c>
@@ -2863,7 +2880,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="27" spans="1:2" ht="31" thickBot="1">
+    <row r="27" spans="1:2" ht="30.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A27" s="14" t="s">
         <v>51</v>
       </c>
@@ -2871,7 +2888,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="28" spans="1:2" ht="19" thickBot="1">
+    <row r="28" spans="1:2" ht="17.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A28" s="14" t="s">
         <v>53</v>
       </c>
@@ -2879,7 +2896,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="29" spans="1:2" ht="15" thickBot="1">
+    <row r="29" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A29" s="14" t="s">
         <v>55</v>
       </c>
@@ -2887,7 +2904,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="30" spans="1:2" ht="15" thickBot="1">
+    <row r="30" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A30" s="14" t="s">
         <v>57</v>
       </c>
@@ -2895,7 +2912,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="31" spans="1:2" ht="69" thickBot="1">
+    <row r="31" spans="1:2" ht="70.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A31" s="14" t="s">
         <v>59</v>
       </c>
@@ -2903,7 +2920,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="32" spans="1:2" ht="21" thickBot="1">
+    <row r="32" spans="1:2" ht="20.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A32" s="14" t="s">
         <v>61</v>
       </c>
@@ -2911,7 +2928,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="33" spans="1:2" ht="15" thickBot="1">
+    <row r="33" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A33" s="14" t="s">
         <v>63</v>
       </c>
@@ -2919,63 +2936,63 @@
         <v>64</v>
       </c>
     </row>
-    <row r="34" spans="1:2">
-      <c r="A34" s="23" t="s">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A34" s="25" t="s">
         <v>65</v>
       </c>
       <c r="B34" s="2" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="35" spans="1:2">
-      <c r="A35" s="25"/>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A35" s="27"/>
       <c r="B35" s="5" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="36" spans="1:2">
-      <c r="A36" s="25"/>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A36" s="27"/>
       <c r="B36" s="5" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="37" spans="1:2">
-      <c r="A37" s="25"/>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A37" s="27"/>
       <c r="B37" s="5" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="38" spans="1:2">
-      <c r="A38" s="25"/>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A38" s="27"/>
       <c r="B38" s="6" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="39" spans="1:2">
-      <c r="A39" s="25"/>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A39" s="27"/>
       <c r="B39" s="6" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="40" spans="1:2">
-      <c r="A40" s="25"/>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A40" s="27"/>
       <c r="B40" s="6" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="41" spans="1:2">
-      <c r="A41" s="25"/>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A41" s="27"/>
       <c r="B41" s="7" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="42" spans="1:2" ht="15" thickBot="1">
-      <c r="A42" s="24"/>
+    <row r="42" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A42" s="26"/>
       <c r="B42" s="8" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="43" spans="1:2">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A43" s="14" t="s">
         <v>75</v>
       </c>
@@ -3000,7 +3017,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr enableFormatConditionsCalculation="0">
+  <sheetPr>
     <tabColor theme="3" tint="0.39997558519241921"/>
   </sheetPr>
   <dimension ref="A1:B50"/>
@@ -3009,13 +3026,13 @@
       <selection activeCell="B40" sqref="B40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="14.1640625" style="15" customWidth="1"/>
-    <col min="2" max="2" width="83.6640625" customWidth="1"/>
+    <col min="1" max="1" width="14.1796875" style="15" customWidth="1"/>
+    <col min="2" max="2" width="83.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15" thickBot="1">
+    <row r="1" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
@@ -3023,7 +3040,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="21" thickBot="1">
+    <row r="2" spans="1:2" ht="20.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="14" t="s">
         <v>77</v>
       </c>
@@ -3031,7 +3048,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="31" thickBot="1">
+    <row r="3" spans="1:2" ht="30.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="14" t="s">
         <v>79</v>
       </c>
@@ -3039,7 +3056,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="29" thickBot="1">
+    <row r="4" spans="1:2" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A4" s="14" t="s">
         <v>81</v>
       </c>
@@ -3047,7 +3064,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="31" thickBot="1">
+    <row r="5" spans="1:2" ht="30.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" s="14" t="s">
         <v>83</v>
       </c>
@@ -3055,21 +3072,21 @@
         <v>84</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="20">
-      <c r="A6" s="23" t="s">
+    <row r="6" spans="1:2" ht="20" x14ac:dyDescent="0.35">
+      <c r="A6" s="25" t="s">
         <v>85</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="15" thickBot="1">
-      <c r="A7" s="24"/>
+    <row r="7" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A7" s="26"/>
       <c r="B7" s="6" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="39" thickBot="1">
+    <row r="8" spans="1:2" ht="37.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A8" s="14" t="s">
         <v>88</v>
       </c>
@@ -3077,7 +3094,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="15" thickBot="1">
+    <row r="9" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A9" s="14" t="s">
         <v>90</v>
       </c>
@@ -3085,7 +3102,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="21" thickBot="1">
+    <row r="10" spans="1:2" ht="20.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A10" s="14" t="s">
         <v>92</v>
       </c>
@@ -3093,7 +3110,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="21" thickBot="1">
+    <row r="11" spans="1:2" ht="20.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A11" s="14" t="s">
         <v>94</v>
       </c>
@@ -3101,7 +3118,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="15" thickBot="1">
+    <row r="12" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A12" s="14" t="s">
         <v>96</v>
       </c>
@@ -3109,7 +3126,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="21" thickBot="1">
+    <row r="13" spans="1:2" ht="20.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A13" s="14" t="s">
         <v>98</v>
       </c>
@@ -3117,7 +3134,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="21" thickBot="1">
+    <row r="14" spans="1:2" ht="20.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A14" s="14" t="s">
         <v>100</v>
       </c>
@@ -3125,7 +3142,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="15" spans="1:2" ht="15" thickBot="1">
+    <row r="15" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A15" s="14" t="s">
         <v>14</v>
       </c>
@@ -3133,7 +3150,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="16" spans="1:2" ht="15" thickBot="1">
+    <row r="16" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A16" s="14" t="s">
         <v>16</v>
       </c>
@@ -3141,7 +3158,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="17" spans="1:2" ht="15" thickBot="1">
+    <row r="17" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A17" s="14" t="s">
         <v>18</v>
       </c>
@@ -3149,7 +3166,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="18" spans="1:2" ht="31" thickBot="1">
+    <row r="18" spans="1:2" ht="30.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A18" s="14" t="s">
         <v>103</v>
       </c>
@@ -3157,7 +3174,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="19" spans="1:2" ht="15" thickBot="1">
+    <row r="19" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A19" s="14" t="s">
         <v>105</v>
       </c>
@@ -3165,7 +3182,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="20" spans="1:2" ht="15" thickBot="1">
+    <row r="20" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A20" s="14" t="s">
         <v>22</v>
       </c>
@@ -3173,7 +3190,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="21" spans="1:2" ht="15" thickBot="1">
+    <row r="21" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A21" s="14" t="s">
         <v>24</v>
       </c>
@@ -3181,7 +3198,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="22" spans="1:2" ht="19" thickBot="1">
+    <row r="22" spans="1:2" ht="17.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A22" s="14" t="s">
         <v>26</v>
       </c>
@@ -3189,97 +3206,97 @@
         <v>107</v>
       </c>
     </row>
-    <row r="23" spans="1:2">
-      <c r="A23" s="23" t="s">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A23" s="25" t="s">
         <v>108</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="24" spans="1:2">
-      <c r="A24" s="25"/>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A24" s="27"/>
       <c r="B24" s="5" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="25" spans="1:2">
-      <c r="A25" s="25"/>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A25" s="27"/>
       <c r="B25" s="5" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="26" spans="1:2">
-      <c r="A26" s="25"/>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A26" s="27"/>
       <c r="B26" s="5" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="27" spans="1:2">
-      <c r="A27" s="25"/>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A27" s="27"/>
       <c r="B27" s="4" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="28" spans="1:2">
-      <c r="A28" s="25"/>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A28" s="27"/>
       <c r="B28" s="3"/>
     </row>
-    <row r="29" spans="1:2">
-      <c r="A29" s="25"/>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A29" s="27"/>
       <c r="B29" s="11" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="30" spans="1:2">
-      <c r="A30" s="25"/>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A30" s="27"/>
       <c r="B30" s="12" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="31" spans="1:2">
-      <c r="A31" s="25"/>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A31" s="27"/>
       <c r="B31" s="6" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="32" spans="1:2">
-      <c r="A32" s="25"/>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A32" s="27"/>
       <c r="B32" s="6" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="33" spans="1:2">
-      <c r="A33" s="25"/>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A33" s="27"/>
       <c r="B33" s="12" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="34" spans="1:2">
-      <c r="A34" s="25"/>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A34" s="27"/>
       <c r="B34" s="6" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="35" spans="1:2">
-      <c r="A35" s="25"/>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A35" s="27"/>
       <c r="B35" s="6" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="36" spans="1:2">
-      <c r="A36" s="25"/>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A36" s="27"/>
       <c r="B36" s="12" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="37" spans="1:2" ht="15" thickBot="1">
-      <c r="A37" s="24"/>
+    <row r="37" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A37" s="26"/>
       <c r="B37" s="6" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="38" spans="1:2" ht="15" thickBot="1">
+    <row r="38" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A38" s="14" t="s">
         <v>28</v>
       </c>
@@ -3287,7 +3304,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="39" spans="1:2" ht="15" thickBot="1">
+    <row r="39" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A39" s="14" t="s">
         <v>30</v>
       </c>
@@ -3295,7 +3312,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="40" spans="1:2" ht="41" thickBot="1">
+    <row r="40" spans="1:2" ht="40.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A40" s="14" t="s">
         <v>125</v>
       </c>
@@ -3303,7 +3320,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="41" spans="1:2" ht="31" thickBot="1">
+    <row r="41" spans="1:2" ht="30.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A41" s="14" t="s">
         <v>127</v>
       </c>
@@ -3311,7 +3328,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="42" spans="1:2" ht="31" thickBot="1">
+    <row r="42" spans="1:2" ht="30.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A42" s="14" t="s">
         <v>129</v>
       </c>
@@ -3319,7 +3336,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="43" spans="1:2" ht="21" thickBot="1">
+    <row r="43" spans="1:2" ht="20.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A43" s="14" t="s">
         <v>41</v>
       </c>
@@ -3327,28 +3344,28 @@
         <v>131</v>
       </c>
     </row>
-    <row r="44" spans="1:2" ht="28">
-      <c r="A44" s="23" t="s">
+    <row r="44" spans="1:2" ht="27" x14ac:dyDescent="0.35">
+      <c r="A44" s="25" t="s">
         <v>132</v>
       </c>
       <c r="B44" s="2" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="45" spans="1:2">
-      <c r="A45" s="25"/>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A45" s="27"/>
       <c r="B45" s="6" t="e">
         <f>--resources="cpus(prod):8; cpus(stage):2 mem(*):15360; disk(*):710534; ports(*):[31000-32000]"</f>
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="46" spans="1:2" ht="15" thickBot="1">
-      <c r="A46" s="24"/>
+    <row r="46" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A46" s="26"/>
       <c r="B46" s="4" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="47" spans="1:2" ht="31" thickBot="1">
+    <row r="47" spans="1:2" ht="30.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A47" s="14" t="s">
         <v>135</v>
       </c>
@@ -3356,7 +3373,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="48" spans="1:2" ht="21" thickBot="1">
+    <row r="48" spans="1:2" ht="20.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A48" s="14" t="s">
         <v>137</v>
       </c>
@@ -3364,7 +3381,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="49" spans="1:2" ht="15" thickBot="1">
+    <row r="49" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A49" s="14" t="s">
         <v>55</v>
       </c>
@@ -3372,7 +3389,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="50" spans="1:2">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A50" s="14" t="s">
         <v>63</v>
       </c>
@@ -3400,27 +3417,27 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr enableFormatConditionsCalculation="0">
+  <sheetPr>
     <tabColor theme="5" tint="0.39997558519241921"/>
   </sheetPr>
   <dimension ref="A1:I43"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B31" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C35" sqref="C35"/>
+      <selection pane="bottomRight" activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="15.5" style="15" customWidth="1"/>
+    <col min="1" max="1" width="15.453125" style="15" customWidth="1"/>
     <col min="2" max="2" width="7" style="15" customWidth="1"/>
     <col min="3" max="3" width="62" customWidth="1"/>
     <col min="4" max="4" width="10" style="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15" thickBot="1">
+    <row r="1" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="13" t="s">
         <v>163</v>
       </c>
@@ -3433,7 +3450,7 @@
       <c r="D1" s="13" t="s">
         <v>141</v>
       </c>
-      <c r="E1" s="36" t="s">
+      <c r="E1" s="23" t="s">
         <v>158</v>
       </c>
       <c r="F1" t="s">
@@ -3449,7 +3466,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="21" thickBot="1">
+    <row r="2" spans="1:9" ht="20.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="14" t="s">
         <v>2</v>
       </c>
@@ -3467,7 +3484,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="41" thickBot="1">
+    <row r="3" spans="1:9" ht="40.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="14" t="s">
         <v>4</v>
       </c>
@@ -3481,11 +3498,11 @@
       <c r="E3" t="s">
         <v>173</v>
       </c>
-      <c r="F3" s="37" t="s">
+      <c r="F3" s="24" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="41" thickBot="1">
+    <row r="4" spans="1:9" ht="50.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A4" s="14" t="s">
         <v>6</v>
       </c>
@@ -3499,11 +3516,11 @@
       <c r="E4" t="s">
         <v>173</v>
       </c>
-      <c r="F4" s="37" t="s">
+      <c r="F4" s="24" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="15" thickBot="1">
+    <row r="5" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" s="14" t="s">
         <v>8</v>
       </c>
@@ -3518,7 +3535,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="61" thickBot="1">
+    <row r="6" spans="1:9" ht="60.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A6" s="14" t="s">
         <v>10</v>
       </c>
@@ -3536,7 +3553,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="21" thickBot="1">
+    <row r="7" spans="1:9" ht="20.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A7" s="14" t="s">
         <v>12</v>
       </c>
@@ -3554,7 +3571,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="21" thickBot="1">
+    <row r="8" spans="1:9" ht="20.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A8" s="14" t="s">
         <v>14</v>
       </c>
@@ -3568,11 +3585,11 @@
       <c r="E8" t="s">
         <v>173</v>
       </c>
-      <c r="F8" s="37" t="s">
+      <c r="F8" s="24" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="21" thickBot="1">
+    <row r="9" spans="1:9" ht="20.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A9" s="14" t="s">
         <v>16</v>
       </c>
@@ -3586,11 +3603,11 @@
       <c r="E9" t="s">
         <v>170</v>
       </c>
-      <c r="F9" s="37" t="s">
+      <c r="F9" s="24" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="15" thickBot="1">
+    <row r="10" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A10" s="14" t="s">
         <v>18</v>
       </c>
@@ -3605,7 +3622,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="31" thickBot="1">
+    <row r="11" spans="1:9" ht="30.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A11" s="14" t="s">
         <v>20</v>
       </c>
@@ -3619,11 +3636,11 @@
       <c r="E11" t="s">
         <v>173</v>
       </c>
-      <c r="F11" s="37" t="s">
+      <c r="F11" s="24" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="21" thickBot="1">
+    <row r="12" spans="1:9" ht="20.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A12" s="14" t="s">
         <v>22</v>
       </c>
@@ -3638,7 +3655,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="15" thickBot="1">
+    <row r="13" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A13" s="14" t="s">
         <v>24</v>
       </c>
@@ -3656,7 +3673,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="21" thickBot="1">
+    <row r="14" spans="1:9" ht="20.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A14" s="14" t="s">
         <v>26</v>
       </c>
@@ -3670,11 +3687,11 @@
       <c r="E14" t="s">
         <v>173</v>
       </c>
-      <c r="F14" s="37" t="s">
+      <c r="F14" s="24" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="15" thickBot="1">
+    <row r="15" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A15" s="14" t="s">
         <v>28</v>
       </c>
@@ -3692,7 +3709,7 @@
         <v>5051</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="15" thickBot="1">
+    <row r="16" spans="1:9" ht="20.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A16" s="14" t="s">
         <v>30</v>
       </c>
@@ -3704,25 +3721,25 @@
         <v>145</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="20.5" customHeight="1">
-      <c r="A17" s="23" t="s">
+    <row r="17" spans="1:4" ht="20.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="25" t="s">
         <v>32</v>
       </c>
       <c r="B17" s="17"/>
-      <c r="C17" s="26" t="s">
+      <c r="C17" s="28" t="s">
         <v>147</v>
       </c>
-      <c r="D17" s="28" t="s">
+      <c r="D17" s="30" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="15" thickBot="1">
-      <c r="A18" s="24"/>
+    <row r="18" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A18" s="26"/>
       <c r="B18" s="18"/>
-      <c r="C18" s="27"/>
-      <c r="D18" s="29"/>
-    </row>
-    <row r="19" spans="1:4" ht="71" thickBot="1">
+      <c r="C18" s="29"/>
+      <c r="D18" s="31"/>
+    </row>
+    <row r="19" spans="1:4" ht="77.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A19" s="14" t="s">
         <v>35</v>
       </c>
@@ -3734,7 +3751,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="21" thickBot="1">
+    <row r="20" spans="1:4" ht="20.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A20" s="14" t="s">
         <v>37</v>
       </c>
@@ -3746,7 +3763,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="21" thickBot="1">
+    <row r="21" spans="1:4" ht="20.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A21" s="14" t="s">
         <v>39</v>
       </c>
@@ -3758,7 +3775,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="21" thickBot="1">
+    <row r="22" spans="1:4" ht="20.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A22" s="14" t="s">
         <v>41</v>
       </c>
@@ -3770,7 +3787,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="21" thickBot="1">
+    <row r="23" spans="1:4" ht="20.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A23" s="14" t="s">
         <v>43</v>
       </c>
@@ -3782,7 +3799,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="41" thickBot="1">
+    <row r="24" spans="1:4" ht="40.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A24" s="14" t="s">
         <v>45</v>
       </c>
@@ -3794,7 +3811,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="19" thickBot="1">
+    <row r="25" spans="1:4" ht="20.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A25" s="14" t="s">
         <v>47</v>
       </c>
@@ -3806,7 +3823,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="21" thickBot="1">
+    <row r="26" spans="1:4" ht="20.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A26" s="14" t="s">
         <v>49</v>
       </c>
@@ -3818,7 +3835,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="41" thickBot="1">
+    <row r="27" spans="1:4" ht="40.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A27" s="14" t="s">
         <v>51</v>
       </c>
@@ -3830,7 +3847,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="21" thickBot="1">
+    <row r="28" spans="1:4" ht="20.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A28" s="14" t="s">
         <v>53</v>
       </c>
@@ -3842,7 +3859,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="15" thickBot="1">
+    <row r="29" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A29" s="14" t="s">
         <v>55</v>
       </c>
@@ -3854,7 +3871,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="21" thickBot="1">
+    <row r="30" spans="1:4" ht="20.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A30" s="14" t="s">
         <v>57</v>
       </c>
@@ -3866,7 +3883,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="89" thickBot="1">
+    <row r="31" spans="1:4" ht="90.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A31" s="14" t="s">
         <v>59</v>
       </c>
@@ -3878,7 +3895,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="21" thickBot="1">
+    <row r="32" spans="1:4" ht="20.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A32" s="14" t="s">
         <v>61</v>
       </c>
@@ -3888,7 +3905,7 @@
       </c>
       <c r="D32" s="16"/>
     </row>
-    <row r="33" spans="1:4" ht="19" thickBot="1">
+    <row r="33" spans="1:4" ht="17.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A33" s="14" t="s">
         <v>63</v>
       </c>
@@ -3900,83 +3917,83 @@
         <v>144</v>
       </c>
     </row>
-    <row r="34" spans="1:4">
-      <c r="A34" s="23" t="s">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A34" s="25" t="s">
         <v>65</v>
       </c>
       <c r="B34" s="17"/>
       <c r="C34" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="D34" s="28" t="s">
+      <c r="D34" s="30" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="35" spans="1:4">
-      <c r="A35" s="25"/>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A35" s="27"/>
       <c r="B35" s="19"/>
       <c r="C35" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="D35" s="30"/>
-    </row>
-    <row r="36" spans="1:4">
-      <c r="A36" s="25"/>
+      <c r="D35" s="32"/>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A36" s="27"/>
       <c r="B36" s="19"/>
       <c r="C36" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="D36" s="30"/>
-    </row>
-    <row r="37" spans="1:4">
-      <c r="A37" s="25"/>
+      <c r="D36" s="32"/>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A37" s="27"/>
       <c r="B37" s="19"/>
       <c r="C37" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="D37" s="30"/>
-    </row>
-    <row r="38" spans="1:4">
-      <c r="A38" s="25"/>
+      <c r="D37" s="32"/>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A38" s="27"/>
       <c r="B38" s="19"/>
       <c r="C38" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="D38" s="30"/>
-    </row>
-    <row r="39" spans="1:4">
-      <c r="A39" s="25"/>
+      <c r="D38" s="32"/>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A39" s="27"/>
       <c r="B39" s="19"/>
       <c r="C39" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="D39" s="30"/>
-    </row>
-    <row r="40" spans="1:4">
-      <c r="A40" s="25"/>
+      <c r="D39" s="32"/>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A40" s="27"/>
       <c r="B40" s="19"/>
       <c r="C40" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="D40" s="30"/>
-    </row>
-    <row r="41" spans="1:4" ht="20">
-      <c r="A41" s="25"/>
+      <c r="D40" s="32"/>
+    </row>
+    <row r="41" spans="1:4" ht="20.5" x14ac:dyDescent="0.35">
+      <c r="A41" s="27"/>
       <c r="B41" s="19"/>
       <c r="C41" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="D41" s="30"/>
-    </row>
-    <row r="42" spans="1:4" ht="15" thickBot="1">
-      <c r="A42" s="24"/>
+      <c r="D41" s="32"/>
+    </row>
+    <row r="42" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A42" s="26"/>
       <c r="B42" s="19"/>
       <c r="C42" s="8" t="s">
         <v>74</v>
       </c>
-      <c r="D42" s="29"/>
-    </row>
-    <row r="43" spans="1:4">
+      <c r="D42" s="31"/>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A43" s="14" t="s">
         <v>75</v>
       </c>
@@ -4004,13 +4021,13 @@
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
-            <xm:f>Sheet3!$B$2:$B$10</xm:f>
+            <xm:f>fileds!$B$2:$B$10</xm:f>
           </x14:formula1>
           <xm:sqref>D1:D1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
-            <xm:f>Sheet3!$D$2:$D$9</xm:f>
+            <xm:f>fileds!$D$2:$D$9</xm:f>
           </x14:formula1>
           <xm:sqref>E1:E1048576</xm:sqref>
         </x14:dataValidation>
@@ -4025,27 +4042,27 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr enableFormatConditionsCalculation="0">
+  <sheetPr>
     <tabColor theme="3" tint="0.39997558519241921"/>
   </sheetPr>
   <dimension ref="A1:H50"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="150" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B26" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E2" sqref="E2"/>
+      <selection pane="bottomRight" activeCell="E41" sqref="E41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="14.1640625" style="15" customWidth="1"/>
-    <col min="2" max="2" width="7.83203125" style="15" customWidth="1"/>
-    <col min="3" max="3" width="83.6640625" customWidth="1"/>
-    <col min="4" max="4" width="8.83203125" style="15"/>
+    <col min="1" max="1" width="14.1796875" style="15" customWidth="1"/>
+    <col min="2" max="2" width="7.81640625" style="15" customWidth="1"/>
+    <col min="3" max="3" width="83.6328125" customWidth="1"/>
+    <col min="4" max="4" width="8.81640625" style="15"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15" thickBot="1">
+    <row r="1" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="13" t="s">
         <v>163</v>
       </c>
@@ -4058,7 +4075,7 @@
       <c r="D1" s="13" t="s">
         <v>141</v>
       </c>
-      <c r="E1" s="36" t="s">
+      <c r="E1" s="23" t="s">
         <v>158</v>
       </c>
       <c r="F1" t="s">
@@ -4071,7 +4088,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="21" thickBot="1">
+    <row r="2" spans="1:8" ht="20.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="14" t="s">
         <v>77</v>
       </c>
@@ -4082,8 +4099,13 @@
       <c r="D2" s="16" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" ht="31" thickBot="1">
+      <c r="E2" s="40" t="s">
+        <v>170</v>
+      </c>
+      <c r="F2" s="40"/>
+      <c r="G2" s="40"/>
+    </row>
+    <row r="3" spans="1:8" ht="30.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="14" t="s">
         <v>79</v>
       </c>
@@ -4094,8 +4116,15 @@
       <c r="D3" s="16" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" ht="29" thickBot="1">
+      <c r="E3" s="40" t="s">
+        <v>175</v>
+      </c>
+      <c r="F3" s="40" t="b">
+        <v>1</v>
+      </c>
+      <c r="G3" s="40"/>
+    </row>
+    <row r="4" spans="1:8" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A4" s="14" t="s">
         <v>81</v>
       </c>
@@ -4106,8 +4135,13 @@
       <c r="D4" s="16" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" ht="31" thickBot="1">
+      <c r="E4" s="40" t="s">
+        <v>170</v>
+      </c>
+      <c r="F4" s="40"/>
+      <c r="G4" s="40"/>
+    </row>
+    <row r="5" spans="1:8" ht="30.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" s="14" t="s">
         <v>83</v>
       </c>
@@ -4118,26 +4152,41 @@
       <c r="D5" s="16" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" ht="20" customHeight="1">
-      <c r="A6" s="31" t="s">
+      <c r="E5" s="40" t="s">
+        <v>172</v>
+      </c>
+      <c r="F5" s="40"/>
+      <c r="G5" s="40"/>
+    </row>
+    <row r="6" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="33" t="s">
         <v>85</v>
       </c>
       <c r="B6" s="20"/>
-      <c r="C6" s="26" t="s">
+      <c r="C6" s="28" t="s">
         <v>152</v>
       </c>
-      <c r="D6" s="28" t="s">
+      <c r="D6" s="35" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" ht="15" thickBot="1">
-      <c r="A7" s="32"/>
+      <c r="E6" s="41" t="s">
+        <v>170</v>
+      </c>
+      <c r="F6" s="41"/>
+      <c r="G6" s="41"/>
+      <c r="H6" s="38"/>
+    </row>
+    <row r="7" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A7" s="34"/>
       <c r="B7" s="21"/>
-      <c r="C7" s="27"/>
-      <c r="D7" s="29"/>
-    </row>
-    <row r="8" spans="1:8" ht="39" thickBot="1">
+      <c r="C7" s="29"/>
+      <c r="D7" s="37"/>
+      <c r="E7" s="41"/>
+      <c r="F7" s="41"/>
+      <c r="G7" s="41"/>
+      <c r="H7" s="38"/>
+    </row>
+    <row r="8" spans="1:8" ht="37.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A8" s="14" t="s">
         <v>88</v>
       </c>
@@ -4145,11 +4194,16 @@
       <c r="C8" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="D8" s="22" t="s">
+      <c r="D8" s="39" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" ht="15" thickBot="1">
+      <c r="E8" s="40" t="s">
+        <v>170</v>
+      </c>
+      <c r="F8" s="40"/>
+      <c r="G8" s="40"/>
+    </row>
+    <row r="9" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A9" s="14" t="s">
         <v>90</v>
       </c>
@@ -4158,8 +4212,15 @@
         <v>91</v>
       </c>
       <c r="D9" s="16"/>
-    </row>
-    <row r="10" spans="1:8" ht="21" thickBot="1">
+      <c r="E9" s="40" t="s">
+        <v>170</v>
+      </c>
+      <c r="F9" s="40" t="s">
+        <v>186</v>
+      </c>
+      <c r="G9" s="40"/>
+    </row>
+    <row r="10" spans="1:8" ht="20.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A10" s="14" t="s">
         <v>92</v>
       </c>
@@ -4170,8 +4231,13 @@
       <c r="D10" s="16" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" ht="21" thickBot="1">
+      <c r="E10" s="40" t="s">
+        <v>170</v>
+      </c>
+      <c r="F10" s="40"/>
+      <c r="G10" s="40"/>
+    </row>
+    <row r="11" spans="1:8" ht="20.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A11" s="14" t="s">
         <v>94</v>
       </c>
@@ -4182,8 +4248,13 @@
       <c r="D11" s="16" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" ht="15" thickBot="1">
+      <c r="E11" s="40" t="s">
+        <v>170</v>
+      </c>
+      <c r="F11" s="40"/>
+      <c r="G11" s="40"/>
+    </row>
+    <row r="12" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A12" s="14" t="s">
         <v>96</v>
       </c>
@@ -4194,8 +4265,13 @@
       <c r="D12" s="16" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" ht="21" thickBot="1">
+      <c r="E12" s="40" t="s">
+        <v>170</v>
+      </c>
+      <c r="F12" s="40"/>
+      <c r="G12" s="40"/>
+    </row>
+    <row r="13" spans="1:8" ht="20.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A13" s="14" t="s">
         <v>98</v>
       </c>
@@ -4206,8 +4282,15 @@
       <c r="D13" s="16" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" ht="21" thickBot="1">
+      <c r="E13" s="40" t="s">
+        <v>170</v>
+      </c>
+      <c r="F13" s="40" t="s">
+        <v>187</v>
+      </c>
+      <c r="G13" s="40"/>
+    </row>
+    <row r="14" spans="1:8" ht="20.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A14" s="14" t="s">
         <v>100</v>
       </c>
@@ -4218,8 +4301,13 @@
       <c r="D14" s="16" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" ht="15" thickBot="1">
+      <c r="E14" s="40" t="s">
+        <v>170</v>
+      </c>
+      <c r="F14" s="40"/>
+      <c r="G14" s="40"/>
+    </row>
+    <row r="15" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A15" s="14" t="s">
         <v>14</v>
       </c>
@@ -4230,8 +4318,15 @@
       <c r="D15" s="16" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" ht="15" thickBot="1">
+      <c r="E15" s="40" t="s">
+        <v>175</v>
+      </c>
+      <c r="F15" s="42" t="s">
+        <v>182</v>
+      </c>
+      <c r="G15" s="40"/>
+    </row>
+    <row r="16" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A16" s="14" t="s">
         <v>16</v>
       </c>
@@ -4242,8 +4337,13 @@
       <c r="D16" s="22" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" ht="15" thickBot="1">
+      <c r="E16" s="40" t="s">
+        <v>170</v>
+      </c>
+      <c r="F16" s="40"/>
+      <c r="G16" s="40"/>
+    </row>
+    <row r="17" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A17" s="14" t="s">
         <v>18</v>
       </c>
@@ -4254,8 +4354,13 @@
       <c r="D17" s="16" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" ht="31" thickBot="1">
+      <c r="E17" s="40" t="s">
+        <v>170</v>
+      </c>
+      <c r="F17" s="40"/>
+      <c r="G17" s="40"/>
+    </row>
+    <row r="18" spans="1:8" ht="30.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A18" s="14" t="s">
         <v>103</v>
       </c>
@@ -4266,8 +4371,13 @@
       <c r="D18" s="16" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" ht="15" thickBot="1">
+      <c r="E18" s="40" t="s">
+        <v>170</v>
+      </c>
+      <c r="F18" s="40"/>
+      <c r="G18" s="40"/>
+    </row>
+    <row r="19" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A19" s="14" t="s">
         <v>105</v>
       </c>
@@ -4278,8 +4388,13 @@
       <c r="D19" s="16" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" ht="15" thickBot="1">
+      <c r="E19" s="40" t="s">
+        <v>170</v>
+      </c>
+      <c r="F19" s="40"/>
+      <c r="G19" s="40"/>
+    </row>
+    <row r="20" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A20" s="14" t="s">
         <v>22</v>
       </c>
@@ -4290,8 +4405,13 @@
       <c r="D20" s="16" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" ht="15" thickBot="1">
+      <c r="E20" s="40" t="s">
+        <v>170</v>
+      </c>
+      <c r="F20" s="40"/>
+      <c r="G20" s="40"/>
+    </row>
+    <row r="21" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A21" s="14" t="s">
         <v>24</v>
       </c>
@@ -4302,8 +4422,15 @@
       <c r="D21" s="16" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" ht="19" thickBot="1">
+      <c r="E21" s="40" t="s">
+        <v>170</v>
+      </c>
+      <c r="F21" s="40">
+        <v>0</v>
+      </c>
+      <c r="G21" s="40"/>
+    </row>
+    <row r="22" spans="1:8" ht="17.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A22" s="14" t="s">
         <v>26</v>
       </c>
@@ -4314,130 +4441,199 @@
       <c r="D22" s="16" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="23" spans="1:4">
-      <c r="A23" s="23" t="s">
+      <c r="E22" s="40" t="s">
+        <v>173</v>
+      </c>
+      <c r="F22" s="40" t="s">
+        <v>185</v>
+      </c>
+      <c r="G22" s="40"/>
+    </row>
+    <row r="23" spans="1:8" ht="20" x14ac:dyDescent="0.35">
+      <c r="A23" s="25" t="s">
         <v>108</v>
       </c>
       <c r="B23" s="17"/>
       <c r="C23" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="D23" s="33" t="s">
+      <c r="D23" s="35" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="24" spans="1:4">
-      <c r="A24" s="25"/>
+      <c r="E23" s="41" t="s">
+        <v>170</v>
+      </c>
+      <c r="F23" s="41"/>
+      <c r="G23" s="41"/>
+      <c r="H23" s="38"/>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A24" s="27"/>
       <c r="B24" s="19"/>
       <c r="C24" s="5" t="s">
         <v>110</v>
       </c>
-      <c r="D24" s="34"/>
-    </row>
-    <row r="25" spans="1:4">
-      <c r="A25" s="25"/>
+      <c r="D24" s="36"/>
+      <c r="E24" s="41"/>
+      <c r="F24" s="41"/>
+      <c r="G24" s="41"/>
+      <c r="H24" s="38"/>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A25" s="27"/>
       <c r="B25" s="19"/>
       <c r="C25" s="5" t="s">
         <v>111</v>
       </c>
-      <c r="D25" s="34"/>
-    </row>
-    <row r="26" spans="1:4">
-      <c r="A26" s="25"/>
+      <c r="D25" s="36"/>
+      <c r="E25" s="41"/>
+      <c r="F25" s="41"/>
+      <c r="G25" s="41"/>
+      <c r="H25" s="38"/>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A26" s="27"/>
       <c r="B26" s="19"/>
       <c r="C26" s="5" t="s">
         <v>112</v>
       </c>
-      <c r="D26" s="34"/>
-    </row>
-    <row r="27" spans="1:4">
-      <c r="A27" s="25"/>
+      <c r="D26" s="36"/>
+      <c r="E26" s="41"/>
+      <c r="F26" s="41"/>
+      <c r="G26" s="41"/>
+      <c r="H26" s="38"/>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A27" s="27"/>
       <c r="B27" s="19"/>
       <c r="C27" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="D27" s="34"/>
-    </row>
-    <row r="28" spans="1:4">
-      <c r="A28" s="25"/>
+      <c r="D27" s="36"/>
+      <c r="E27" s="41"/>
+      <c r="F27" s="41"/>
+      <c r="G27" s="41"/>
+      <c r="H27" s="38"/>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A28" s="27"/>
       <c r="B28" s="19"/>
       <c r="C28" s="3"/>
-      <c r="D28" s="34"/>
-    </row>
-    <row r="29" spans="1:4">
-      <c r="A29" s="25"/>
+      <c r="D28" s="36"/>
+      <c r="E28" s="41"/>
+      <c r="F28" s="41"/>
+      <c r="G28" s="41"/>
+      <c r="H28" s="38"/>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A29" s="27"/>
       <c r="B29" s="19"/>
       <c r="C29" s="11" t="s">
         <v>114</v>
       </c>
-      <c r="D29" s="34"/>
-    </row>
-    <row r="30" spans="1:4">
-      <c r="A30" s="25"/>
+      <c r="D29" s="36"/>
+      <c r="E29" s="41"/>
+      <c r="F29" s="41"/>
+      <c r="G29" s="41"/>
+      <c r="H29" s="38"/>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A30" s="27"/>
       <c r="B30" s="19"/>
       <c r="C30" s="12" t="s">
         <v>115</v>
       </c>
-      <c r="D30" s="34"/>
-    </row>
-    <row r="31" spans="1:4">
-      <c r="A31" s="25"/>
+      <c r="D30" s="36"/>
+      <c r="E30" s="41"/>
+      <c r="F30" s="41"/>
+      <c r="G30" s="41"/>
+      <c r="H30" s="38"/>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A31" s="27"/>
       <c r="B31" s="19"/>
       <c r="C31" s="6" t="s">
         <v>116</v>
       </c>
-      <c r="D31" s="34"/>
-    </row>
-    <row r="32" spans="1:4">
-      <c r="A32" s="25"/>
+      <c r="D31" s="36"/>
+      <c r="E31" s="41"/>
+      <c r="F31" s="41"/>
+      <c r="G31" s="41"/>
+      <c r="H31" s="38"/>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A32" s="27"/>
       <c r="B32" s="19"/>
       <c r="C32" s="6" t="s">
         <v>117</v>
       </c>
-      <c r="D32" s="34"/>
-    </row>
-    <row r="33" spans="1:4">
-      <c r="A33" s="25"/>
+      <c r="D32" s="36"/>
+      <c r="E32" s="41"/>
+      <c r="F32" s="41"/>
+      <c r="G32" s="41"/>
+      <c r="H32" s="38"/>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A33" s="27"/>
       <c r="B33" s="19"/>
       <c r="C33" s="12" t="s">
         <v>118</v>
       </c>
-      <c r="D33" s="34"/>
-    </row>
-    <row r="34" spans="1:4">
-      <c r="A34" s="25"/>
+      <c r="D33" s="36"/>
+      <c r="E33" s="41"/>
+      <c r="F33" s="41"/>
+      <c r="G33" s="41"/>
+      <c r="H33" s="38"/>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A34" s="27"/>
       <c r="B34" s="19"/>
       <c r="C34" s="6" t="s">
         <v>119</v>
       </c>
-      <c r="D34" s="34"/>
-    </row>
-    <row r="35" spans="1:4">
-      <c r="A35" s="25"/>
+      <c r="D34" s="36"/>
+      <c r="E34" s="41"/>
+      <c r="F34" s="41"/>
+      <c r="G34" s="41"/>
+      <c r="H34" s="38"/>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A35" s="27"/>
       <c r="B35" s="19"/>
       <c r="C35" s="6" t="s">
         <v>120</v>
       </c>
-      <c r="D35" s="34"/>
-    </row>
-    <row r="36" spans="1:4">
-      <c r="A36" s="25"/>
+      <c r="D35" s="36"/>
+      <c r="E35" s="41"/>
+      <c r="F35" s="41"/>
+      <c r="G35" s="41"/>
+      <c r="H35" s="38"/>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A36" s="27"/>
       <c r="B36" s="19"/>
       <c r="C36" s="12" t="s">
         <v>121</v>
       </c>
-      <c r="D36" s="34"/>
-    </row>
-    <row r="37" spans="1:4" ht="15" thickBot="1">
-      <c r="A37" s="24"/>
+      <c r="D36" s="36"/>
+      <c r="E36" s="41"/>
+      <c r="F36" s="41"/>
+      <c r="G36" s="41"/>
+      <c r="H36" s="38"/>
+    </row>
+    <row r="37" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A37" s="26"/>
       <c r="B37" s="19"/>
       <c r="C37" s="6" t="s">
         <v>122</v>
       </c>
-      <c r="D37" s="35"/>
-    </row>
-    <row r="38" spans="1:4" ht="15" thickBot="1">
+      <c r="D37" s="37"/>
+      <c r="E37" s="41"/>
+      <c r="F37" s="41"/>
+      <c r="G37" s="41"/>
+      <c r="H37" s="38"/>
+    </row>
+    <row r="38" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A38" s="14" t="s">
         <v>28</v>
       </c>
@@ -4448,8 +4644,15 @@
       <c r="D38" s="16" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="39" spans="1:4" ht="15" thickBot="1">
+      <c r="E38" s="40" t="s">
+        <v>170</v>
+      </c>
+      <c r="F38" s="40">
+        <v>5051</v>
+      </c>
+      <c r="G38" s="40"/>
+    </row>
+    <row r="39" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A39" s="14" t="s">
         <v>30</v>
       </c>
@@ -4460,8 +4663,11 @@
       <c r="D39" s="16" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="40" spans="1:4" ht="41" thickBot="1">
+      <c r="E39" s="40"/>
+      <c r="F39" s="40"/>
+      <c r="G39" s="40"/>
+    </row>
+    <row r="40" spans="1:8" ht="40.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A40" s="14" t="s">
         <v>125</v>
       </c>
@@ -4472,8 +4678,13 @@
       <c r="D40" s="16" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="41" spans="1:4" ht="31" thickBot="1">
+      <c r="E40" s="40" t="s">
+        <v>175</v>
+      </c>
+      <c r="F40" s="40"/>
+      <c r="G40" s="40"/>
+    </row>
+    <row r="41" spans="1:8" ht="30.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A41" s="14" t="s">
         <v>127</v>
       </c>
@@ -4484,8 +4695,11 @@
       <c r="D41" s="16" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="42" spans="1:4" ht="31" thickBot="1">
+      <c r="E41" s="40"/>
+      <c r="F41" s="40"/>
+      <c r="G41" s="40"/>
+    </row>
+    <row r="42" spans="1:8" ht="40.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A42" s="14" t="s">
         <v>129</v>
       </c>
@@ -4494,8 +4708,11 @@
         <v>130</v>
       </c>
       <c r="D42" s="16"/>
-    </row>
-    <row r="43" spans="1:4" ht="21" thickBot="1">
+      <c r="E42" s="40"/>
+      <c r="F42" s="40"/>
+      <c r="G42" s="40"/>
+    </row>
+    <row r="43" spans="1:8" ht="20.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A43" s="14" t="s">
         <v>41</v>
       </c>
@@ -4506,37 +4723,52 @@
       <c r="D43" s="16" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="44" spans="1:4" ht="28">
-      <c r="A44" s="23" t="s">
+      <c r="E43" s="40"/>
+      <c r="F43" s="40"/>
+      <c r="G43" s="40"/>
+    </row>
+    <row r="44" spans="1:8" ht="27" x14ac:dyDescent="0.35">
+      <c r="A44" s="25" t="s">
         <v>132</v>
       </c>
       <c r="B44" s="17"/>
       <c r="C44" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="D44" s="33" t="s">
+      <c r="D44" s="35" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="45" spans="1:4">
-      <c r="A45" s="25"/>
+      <c r="E44" s="41"/>
+      <c r="F44" s="41"/>
+      <c r="G44" s="41"/>
+      <c r="H44" s="38"/>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A45" s="27"/>
       <c r="B45" s="19"/>
       <c r="C45" s="6" t="e">
         <f>--resources="cpus(prod):8; cpus(stage):2 mem(*):15360; disk(*):710534; ports(*):[31000-32000]"</f>
         <v>#VALUE!</v>
       </c>
-      <c r="D45" s="34"/>
-    </row>
-    <row r="46" spans="1:4" ht="15" thickBot="1">
-      <c r="A46" s="24"/>
+      <c r="D45" s="36"/>
+      <c r="E45" s="41"/>
+      <c r="F45" s="41"/>
+      <c r="G45" s="41"/>
+      <c r="H45" s="38"/>
+    </row>
+    <row r="46" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A46" s="26"/>
       <c r="B46" s="19"/>
       <c r="C46" s="4" t="s">
         <v>134</v>
       </c>
-      <c r="D46" s="35"/>
-    </row>
-    <row r="47" spans="1:4" ht="31" thickBot="1">
+      <c r="D46" s="37"/>
+      <c r="E46" s="41"/>
+      <c r="F46" s="41"/>
+      <c r="G46" s="41"/>
+      <c r="H46" s="38"/>
+    </row>
+    <row r="47" spans="1:8" ht="30.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A47" s="14" t="s">
         <v>135</v>
       </c>
@@ -4547,8 +4779,15 @@
       <c r="D47" s="16" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="48" spans="1:4" ht="21" thickBot="1">
+      <c r="E47" s="40" t="s">
+        <v>175</v>
+      </c>
+      <c r="F47" s="42" t="s">
+        <v>191</v>
+      </c>
+      <c r="G47" s="40"/>
+    </row>
+    <row r="48" spans="1:8" ht="20.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A48" s="14" t="s">
         <v>137</v>
       </c>
@@ -4559,8 +4798,15 @@
       <c r="D48" s="16" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="49" spans="1:4" ht="15" thickBot="1">
+      <c r="E48" s="40" t="s">
+        <v>189</v>
+      </c>
+      <c r="F48" s="42" t="s">
+        <v>190</v>
+      </c>
+      <c r="G48" s="40"/>
+    </row>
+    <row r="49" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A49" s="14" t="s">
         <v>55</v>
       </c>
@@ -4571,8 +4817,15 @@
       <c r="D49" s="16" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="50" spans="1:4">
+      <c r="E49" s="40" t="s">
+        <v>175</v>
+      </c>
+      <c r="F49" s="42" t="s">
+        <v>188</v>
+      </c>
+      <c r="G49" s="40"/>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A50" s="14" t="s">
         <v>63</v>
       </c>
@@ -4583,9 +4836,26 @@
       <c r="D50" s="16" t="s">
         <v>144</v>
       </c>
+      <c r="E50" s="40" t="s">
+        <v>170</v>
+      </c>
+      <c r="F50" s="40"/>
+      <c r="G50" s="40"/>
     </row>
   </sheetData>
-  <mergeCells count="7">
+  <mergeCells count="19">
+    <mergeCell ref="E44:E46"/>
+    <mergeCell ref="F44:F46"/>
+    <mergeCell ref="G44:G46"/>
+    <mergeCell ref="H44:H46"/>
+    <mergeCell ref="E6:E7"/>
+    <mergeCell ref="F6:F7"/>
+    <mergeCell ref="G6:G7"/>
+    <mergeCell ref="H6:H7"/>
+    <mergeCell ref="E23:E37"/>
+    <mergeCell ref="F23:F37"/>
+    <mergeCell ref="G23:G37"/>
+    <mergeCell ref="H23:H37"/>
     <mergeCell ref="A6:A7"/>
     <mergeCell ref="A23:A37"/>
     <mergeCell ref="A44:A46"/>
@@ -4598,21 +4868,21 @@
     <hyperlink ref="C4" r:id="rId1" location="containerizer" display="https://open.mesosphere.com/reference/glossary/ - containerizer"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
-            <xm:f>Sheet3!$C$2:$C$10</xm:f>
+            <xm:f>fileds!$C$2:$C$10</xm:f>
           </x14:formula1>
           <xm:sqref>D1:D1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
-            <xm:f>Sheet3!$D$2:$D$9</xm:f>
+            <xm:f>fileds!$D$2:$D$9</xm:f>
           </x14:formula1>
-          <xm:sqref>E1:E1048576</xm:sqref>
+          <xm:sqref>E1:E6 E8:E23 E38:E44 E47:E1048576</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -4628,12 +4898,12 @@
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="J40" sqref="J40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>165</v>
       </c>
@@ -4647,7 +4917,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>153</v>
       </c>
@@ -4661,7 +4931,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>154</v>
       </c>
@@ -4675,7 +4945,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>155</v>
       </c>
@@ -4689,7 +4959,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>156</v>
       </c>
@@ -4703,7 +4973,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>157</v>
       </c>
@@ -4717,7 +4987,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B7" t="s">
         <v>148</v>
       </c>
@@ -4728,7 +4998,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B8" t="s">
         <v>37</v>
       </c>
@@ -4739,7 +5009,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B9" t="s">
         <v>146</v>
       </c>
@@ -4750,7 +5020,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B10" t="s">
         <v>142</v>
       </c>

</xml_diff>

<commit_message>
add more UI Type for agent
</commit_message>
<xml_diff>
--- a/configuration flags.xlsx
+++ b/configuration flags.xlsx
@@ -130,7 +130,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="480" uniqueCount="192">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="487" uniqueCount="194">
   <si>
     <t>Flag</t>
   </si>
@@ -2062,6 +2062,12 @@
   </si>
   <si>
     <t>--strict</t>
+  </si>
+  <si>
+    <t>15 mins</t>
+  </si>
+  <si>
+    <t>1 secs</t>
   </si>
 </sst>
 </file>
@@ -2295,6 +2301,11 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -2319,6 +2330,12 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2328,23 +2345,12 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="11">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -2415,7 +2421,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2450,7 +2456,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2803,7 +2809,7 @@
       </c>
     </row>
     <row r="17" spans="1:2" ht="20" x14ac:dyDescent="0.35">
-      <c r="A17" s="25" t="s">
+      <c r="A17" s="28" t="s">
         <v>32</v>
       </c>
       <c r="B17" s="2" t="s">
@@ -2811,7 +2817,7 @@
       </c>
     </row>
     <row r="18" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A18" s="26"/>
+      <c r="A18" s="29"/>
       <c r="B18" s="4" t="s">
         <v>34</v>
       </c>
@@ -2937,7 +2943,7 @@
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A34" s="25" t="s">
+      <c r="A34" s="28" t="s">
         <v>65</v>
       </c>
       <c r="B34" s="2" t="s">
@@ -2945,49 +2951,49 @@
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A35" s="27"/>
+      <c r="A35" s="30"/>
       <c r="B35" s="5" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A36" s="27"/>
+      <c r="A36" s="30"/>
       <c r="B36" s="5" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A37" s="27"/>
+      <c r="A37" s="30"/>
       <c r="B37" s="5" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A38" s="27"/>
+      <c r="A38" s="30"/>
       <c r="B38" s="6" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A39" s="27"/>
+      <c r="A39" s="30"/>
       <c r="B39" s="6" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A40" s="27"/>
+      <c r="A40" s="30"/>
       <c r="B40" s="6" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A41" s="27"/>
+      <c r="A41" s="30"/>
       <c r="B41" s="7" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="42" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A42" s="26"/>
+      <c r="A42" s="29"/>
       <c r="B42" s="8" t="s">
         <v>74</v>
       </c>
@@ -3073,7 +3079,7 @@
       </c>
     </row>
     <row r="6" spans="1:2" ht="20" x14ac:dyDescent="0.35">
-      <c r="A6" s="25" t="s">
+      <c r="A6" s="28" t="s">
         <v>85</v>
       </c>
       <c r="B6" s="2" t="s">
@@ -3081,7 +3087,7 @@
       </c>
     </row>
     <row r="7" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="26"/>
+      <c r="A7" s="29"/>
       <c r="B7" s="6" t="s">
         <v>87</v>
       </c>
@@ -3207,7 +3213,7 @@
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A23" s="25" t="s">
+      <c r="A23" s="28" t="s">
         <v>108</v>
       </c>
       <c r="B23" s="2" t="s">
@@ -3215,83 +3221,83 @@
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A24" s="27"/>
+      <c r="A24" s="30"/>
       <c r="B24" s="5" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A25" s="27"/>
+      <c r="A25" s="30"/>
       <c r="B25" s="5" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A26" s="27"/>
+      <c r="A26" s="30"/>
       <c r="B26" s="5" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A27" s="27"/>
+      <c r="A27" s="30"/>
       <c r="B27" s="4" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A28" s="27"/>
+      <c r="A28" s="30"/>
       <c r="B28" s="3"/>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A29" s="27"/>
+      <c r="A29" s="30"/>
       <c r="B29" s="11" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A30" s="27"/>
+      <c r="A30" s="30"/>
       <c r="B30" s="12" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A31" s="27"/>
+      <c r="A31" s="30"/>
       <c r="B31" s="6" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A32" s="27"/>
+      <c r="A32" s="30"/>
       <c r="B32" s="6" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A33" s="27"/>
+      <c r="A33" s="30"/>
       <c r="B33" s="12" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A34" s="27"/>
+      <c r="A34" s="30"/>
       <c r="B34" s="6" t="s">
         <v>119</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A35" s="27"/>
+      <c r="A35" s="30"/>
       <c r="B35" s="6" t="s">
         <v>120</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A36" s="27"/>
+      <c r="A36" s="30"/>
       <c r="B36" s="12" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A37" s="26"/>
+      <c r="A37" s="29"/>
       <c r="B37" s="6" t="s">
         <v>122</v>
       </c>
@@ -3345,7 +3351,7 @@
       </c>
     </row>
     <row r="44" spans="1:2" ht="27" x14ac:dyDescent="0.35">
-      <c r="A44" s="25" t="s">
+      <c r="A44" s="28" t="s">
         <v>132</v>
       </c>
       <c r="B44" s="2" t="s">
@@ -3353,14 +3359,14 @@
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A45" s="27"/>
+      <c r="A45" s="30"/>
       <c r="B45" s="6" t="e">
         <f>--resources="cpus(prod):8; cpus(stage):2 mem(*):15360; disk(*):710534; ports(*):[31000-32000]"</f>
         <v>#VALUE!</v>
       </c>
     </row>
     <row r="46" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A46" s="26"/>
+      <c r="A46" s="29"/>
       <c r="B46" s="4" t="s">
         <v>134</v>
       </c>
@@ -3722,22 +3728,22 @@
       </c>
     </row>
     <row r="17" spans="1:4" ht="20.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="25" t="s">
+      <c r="A17" s="28" t="s">
         <v>32</v>
       </c>
       <c r="B17" s="17"/>
-      <c r="C17" s="28" t="s">
+      <c r="C17" s="31" t="s">
         <v>147</v>
       </c>
-      <c r="D17" s="30" t="s">
+      <c r="D17" s="33" t="s">
         <v>146</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A18" s="26"/>
+      <c r="A18" s="29"/>
       <c r="B18" s="18"/>
-      <c r="C18" s="29"/>
-      <c r="D18" s="31"/>
+      <c r="C18" s="32"/>
+      <c r="D18" s="34"/>
     </row>
     <row r="19" spans="1:4" ht="77.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A19" s="14" t="s">
@@ -3918,80 +3924,80 @@
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A34" s="25" t="s">
+      <c r="A34" s="28" t="s">
         <v>65</v>
       </c>
       <c r="B34" s="17"/>
       <c r="C34" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="D34" s="30" t="s">
+      <c r="D34" s="33" t="s">
         <v>146</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A35" s="27"/>
+      <c r="A35" s="30"/>
       <c r="B35" s="19"/>
       <c r="C35" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="D35" s="32"/>
+      <c r="D35" s="35"/>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A36" s="27"/>
+      <c r="A36" s="30"/>
       <c r="B36" s="19"/>
       <c r="C36" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="D36" s="32"/>
+      <c r="D36" s="35"/>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A37" s="27"/>
+      <c r="A37" s="30"/>
       <c r="B37" s="19"/>
       <c r="C37" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="D37" s="32"/>
+      <c r="D37" s="35"/>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A38" s="27"/>
+      <c r="A38" s="30"/>
       <c r="B38" s="19"/>
       <c r="C38" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="D38" s="32"/>
+      <c r="D38" s="35"/>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A39" s="27"/>
+      <c r="A39" s="30"/>
       <c r="B39" s="19"/>
       <c r="C39" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="D39" s="32"/>
+      <c r="D39" s="35"/>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A40" s="27"/>
+      <c r="A40" s="30"/>
       <c r="B40" s="19"/>
       <c r="C40" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="D40" s="32"/>
+      <c r="D40" s="35"/>
     </row>
     <row r="41" spans="1:4" ht="20.5" x14ac:dyDescent="0.35">
-      <c r="A41" s="27"/>
+      <c r="A41" s="30"/>
       <c r="B41" s="19"/>
       <c r="C41" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="D41" s="32"/>
+      <c r="D41" s="35"/>
     </row>
     <row r="42" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A42" s="26"/>
+      <c r="A42" s="29"/>
       <c r="B42" s="19"/>
       <c r="C42" s="8" t="s">
         <v>74</v>
       </c>
-      <c r="D42" s="31"/>
+      <c r="D42" s="34"/>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A43" s="14" t="s">
@@ -4048,10 +4054,10 @@
   <dimension ref="A1:H50"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="150" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B26" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E41" sqref="E41"/>
+      <selection pane="bottomRight" activeCell="F44" sqref="F44:F46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4099,11 +4105,11 @@
       <c r="D2" s="16" t="s">
         <v>150</v>
       </c>
-      <c r="E2" s="40" t="s">
+      <c r="E2" s="26" t="s">
         <v>170</v>
       </c>
-      <c r="F2" s="40"/>
-      <c r="G2" s="40"/>
+      <c r="F2" s="26"/>
+      <c r="G2" s="26"/>
     </row>
     <row r="3" spans="1:8" ht="30.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="14" t="s">
@@ -4116,13 +4122,13 @@
       <c r="D3" s="16" t="s">
         <v>142</v>
       </c>
-      <c r="E3" s="40" t="s">
+      <c r="E3" s="26" t="s">
         <v>175</v>
       </c>
-      <c r="F3" s="40" t="b">
+      <c r="F3" s="26" t="b">
         <v>1</v>
       </c>
-      <c r="G3" s="40"/>
+      <c r="G3" s="26"/>
     </row>
     <row r="4" spans="1:8" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A4" s="14" t="s">
@@ -4135,11 +4141,11 @@
       <c r="D4" s="16" t="s">
         <v>151</v>
       </c>
-      <c r="E4" s="40" t="s">
+      <c r="E4" s="26" t="s">
         <v>170</v>
       </c>
-      <c r="F4" s="40"/>
-      <c r="G4" s="40"/>
+      <c r="F4" s="26"/>
+      <c r="G4" s="26"/>
     </row>
     <row r="5" spans="1:8" ht="30.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" s="14" t="s">
@@ -4152,39 +4158,39 @@
       <c r="D5" s="16" t="s">
         <v>142</v>
       </c>
-      <c r="E5" s="40" t="s">
+      <c r="E5" s="26" t="s">
         <v>172</v>
       </c>
-      <c r="F5" s="40"/>
-      <c r="G5" s="40"/>
+      <c r="F5" s="26"/>
+      <c r="G5" s="26"/>
     </row>
     <row r="6" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="33" t="s">
+      <c r="A6" s="38" t="s">
         <v>85</v>
       </c>
       <c r="B6" s="20"/>
-      <c r="C6" s="28" t="s">
+      <c r="C6" s="31" t="s">
         <v>152</v>
       </c>
-      <c r="D6" s="35" t="s">
+      <c r="D6" s="40" t="s">
         <v>151</v>
       </c>
-      <c r="E6" s="41" t="s">
+      <c r="E6" s="36" t="s">
         <v>170</v>
       </c>
-      <c r="F6" s="41"/>
-      <c r="G6" s="41"/>
-      <c r="H6" s="38"/>
+      <c r="F6" s="36"/>
+      <c r="G6" s="36"/>
+      <c r="H6" s="37"/>
     </row>
     <row r="7" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="34"/>
+      <c r="A7" s="39"/>
       <c r="B7" s="21"/>
-      <c r="C7" s="29"/>
-      <c r="D7" s="37"/>
-      <c r="E7" s="41"/>
-      <c r="F7" s="41"/>
-      <c r="G7" s="41"/>
-      <c r="H7" s="38"/>
+      <c r="C7" s="32"/>
+      <c r="D7" s="41"/>
+      <c r="E7" s="36"/>
+      <c r="F7" s="36"/>
+      <c r="G7" s="36"/>
+      <c r="H7" s="37"/>
     </row>
     <row r="8" spans="1:8" ht="37.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A8" s="14" t="s">
@@ -4194,14 +4200,14 @@
       <c r="C8" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="D8" s="39" t="s">
+      <c r="D8" s="25" t="s">
         <v>143</v>
       </c>
-      <c r="E8" s="40" t="s">
+      <c r="E8" s="26" t="s">
         <v>170</v>
       </c>
-      <c r="F8" s="40"/>
-      <c r="G8" s="40"/>
+      <c r="F8" s="26"/>
+      <c r="G8" s="26"/>
     </row>
     <row r="9" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A9" s="14" t="s">
@@ -4212,13 +4218,13 @@
         <v>91</v>
       </c>
       <c r="D9" s="16"/>
-      <c r="E9" s="40" t="s">
+      <c r="E9" s="26" t="s">
         <v>170</v>
       </c>
-      <c r="F9" s="40" t="s">
+      <c r="F9" s="26" t="s">
         <v>186</v>
       </c>
-      <c r="G9" s="40"/>
+      <c r="G9" s="26"/>
     </row>
     <row r="10" spans="1:8" ht="20.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A10" s="14" t="s">
@@ -4231,11 +4237,11 @@
       <c r="D10" s="16" t="s">
         <v>143</v>
       </c>
-      <c r="E10" s="40" t="s">
+      <c r="E10" s="26" t="s">
         <v>170</v>
       </c>
-      <c r="F10" s="40"/>
-      <c r="G10" s="40"/>
+      <c r="F10" s="26"/>
+      <c r="G10" s="26"/>
     </row>
     <row r="11" spans="1:8" ht="20.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A11" s="14" t="s">
@@ -4248,11 +4254,11 @@
       <c r="D11" s="16" t="s">
         <v>143</v>
       </c>
-      <c r="E11" s="40" t="s">
+      <c r="E11" s="26" t="s">
         <v>170</v>
       </c>
-      <c r="F11" s="40"/>
-      <c r="G11" s="40"/>
+      <c r="F11" s="26"/>
+      <c r="G11" s="26"/>
     </row>
     <row r="12" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A12" s="14" t="s">
@@ -4265,11 +4271,11 @@
       <c r="D12" s="16" t="s">
         <v>143</v>
       </c>
-      <c r="E12" s="40" t="s">
+      <c r="E12" s="26" t="s">
         <v>170</v>
       </c>
-      <c r="F12" s="40"/>
-      <c r="G12" s="40"/>
+      <c r="F12" s="26"/>
+      <c r="G12" s="26"/>
     </row>
     <row r="13" spans="1:8" ht="20.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A13" s="14" t="s">
@@ -4282,13 +4288,13 @@
       <c r="D13" s="16" t="s">
         <v>143</v>
       </c>
-      <c r="E13" s="40" t="s">
+      <c r="E13" s="26" t="s">
         <v>170</v>
       </c>
-      <c r="F13" s="40" t="s">
+      <c r="F13" s="26" t="s">
         <v>187</v>
       </c>
-      <c r="G13" s="40"/>
+      <c r="G13" s="26"/>
     </row>
     <row r="14" spans="1:8" ht="20.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A14" s="14" t="s">
@@ -4301,11 +4307,11 @@
       <c r="D14" s="16" t="s">
         <v>143</v>
       </c>
-      <c r="E14" s="40" t="s">
+      <c r="E14" s="26" t="s">
         <v>170</v>
       </c>
-      <c r="F14" s="40"/>
-      <c r="G14" s="40"/>
+      <c r="F14" s="26"/>
+      <c r="G14" s="26"/>
     </row>
     <row r="15" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A15" s="14" t="s">
@@ -4318,13 +4324,13 @@
       <c r="D15" s="16" t="s">
         <v>144</v>
       </c>
-      <c r="E15" s="40" t="s">
+      <c r="E15" s="26" t="s">
         <v>175</v>
       </c>
-      <c r="F15" s="42" t="s">
+      <c r="F15" s="27" t="s">
         <v>182</v>
       </c>
-      <c r="G15" s="40"/>
+      <c r="G15" s="26"/>
     </row>
     <row r="16" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A16" s="14" t="s">
@@ -4337,11 +4343,11 @@
       <c r="D16" s="22" t="s">
         <v>144</v>
       </c>
-      <c r="E16" s="40" t="s">
+      <c r="E16" s="26" t="s">
         <v>170</v>
       </c>
-      <c r="F16" s="40"/>
-      <c r="G16" s="40"/>
+      <c r="F16" s="26"/>
+      <c r="G16" s="26"/>
     </row>
     <row r="17" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A17" s="14" t="s">
@@ -4354,11 +4360,11 @@
       <c r="D17" s="16" t="s">
         <v>144</v>
       </c>
-      <c r="E17" s="40" t="s">
+      <c r="E17" s="26" t="s">
         <v>170</v>
       </c>
-      <c r="F17" s="40"/>
-      <c r="G17" s="40"/>
+      <c r="F17" s="26"/>
+      <c r="G17" s="26"/>
     </row>
     <row r="18" spans="1:8" ht="30.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A18" s="14" t="s">
@@ -4371,11 +4377,11 @@
       <c r="D18" s="16" t="s">
         <v>144</v>
       </c>
-      <c r="E18" s="40" t="s">
+      <c r="E18" s="26" t="s">
         <v>170</v>
       </c>
-      <c r="F18" s="40"/>
-      <c r="G18" s="40"/>
+      <c r="F18" s="26"/>
+      <c r="G18" s="26"/>
     </row>
     <row r="19" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A19" s="14" t="s">
@@ -4388,11 +4394,11 @@
       <c r="D19" s="16" t="s">
         <v>144</v>
       </c>
-      <c r="E19" s="40" t="s">
+      <c r="E19" s="26" t="s">
         <v>170</v>
       </c>
-      <c r="F19" s="40"/>
-      <c r="G19" s="40"/>
+      <c r="F19" s="26"/>
+      <c r="G19" s="26"/>
     </row>
     <row r="20" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A20" s="14" t="s">
@@ -4405,11 +4411,11 @@
       <c r="D20" s="16" t="s">
         <v>145</v>
       </c>
-      <c r="E20" s="40" t="s">
+      <c r="E20" s="26" t="s">
         <v>170</v>
       </c>
-      <c r="F20" s="40"/>
-      <c r="G20" s="40"/>
+      <c r="F20" s="26"/>
+      <c r="G20" s="26"/>
     </row>
     <row r="21" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A21" s="14" t="s">
@@ -4422,13 +4428,13 @@
       <c r="D21" s="16" t="s">
         <v>145</v>
       </c>
-      <c r="E21" s="40" t="s">
+      <c r="E21" s="26" t="s">
         <v>170</v>
       </c>
-      <c r="F21" s="40">
+      <c r="F21" s="26">
         <v>0</v>
       </c>
-      <c r="G21" s="40"/>
+      <c r="G21" s="26"/>
     </row>
     <row r="22" spans="1:8" ht="17.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A22" s="14" t="s">
@@ -4441,197 +4447,197 @@
       <c r="D22" s="16" t="s">
         <v>145</v>
       </c>
-      <c r="E22" s="40" t="s">
+      <c r="E22" s="26" t="s">
         <v>173</v>
       </c>
-      <c r="F22" s="40" t="s">
+      <c r="F22" s="26" t="s">
         <v>185</v>
       </c>
-      <c r="G22" s="40"/>
-    </row>
-    <row r="23" spans="1:8" ht="20" x14ac:dyDescent="0.35">
-      <c r="A23" s="25" t="s">
+      <c r="G22" s="26"/>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A23" s="28" t="s">
         <v>108</v>
       </c>
       <c r="B23" s="17"/>
       <c r="C23" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="D23" s="35" t="s">
+      <c r="D23" s="40" t="s">
         <v>144</v>
       </c>
-      <c r="E23" s="41" t="s">
+      <c r="E23" s="36" t="s">
         <v>170</v>
       </c>
-      <c r="F23" s="41"/>
-      <c r="G23" s="41"/>
-      <c r="H23" s="38"/>
+      <c r="F23" s="36"/>
+      <c r="G23" s="36"/>
+      <c r="H23" s="37"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A24" s="27"/>
+      <c r="A24" s="30"/>
       <c r="B24" s="19"/>
       <c r="C24" s="5" t="s">
         <v>110</v>
       </c>
-      <c r="D24" s="36"/>
-      <c r="E24" s="41"/>
-      <c r="F24" s="41"/>
-      <c r="G24" s="41"/>
-      <c r="H24" s="38"/>
+      <c r="D24" s="42"/>
+      <c r="E24" s="36"/>
+      <c r="F24" s="36"/>
+      <c r="G24" s="36"/>
+      <c r="H24" s="37"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A25" s="27"/>
+      <c r="A25" s="30"/>
       <c r="B25" s="19"/>
       <c r="C25" s="5" t="s">
         <v>111</v>
       </c>
-      <c r="D25" s="36"/>
-      <c r="E25" s="41"/>
-      <c r="F25" s="41"/>
-      <c r="G25" s="41"/>
-      <c r="H25" s="38"/>
+      <c r="D25" s="42"/>
+      <c r="E25" s="36"/>
+      <c r="F25" s="36"/>
+      <c r="G25" s="36"/>
+      <c r="H25" s="37"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A26" s="27"/>
+      <c r="A26" s="30"/>
       <c r="B26" s="19"/>
       <c r="C26" s="5" t="s">
         <v>112</v>
       </c>
-      <c r="D26" s="36"/>
-      <c r="E26" s="41"/>
-      <c r="F26" s="41"/>
-      <c r="G26" s="41"/>
-      <c r="H26" s="38"/>
+      <c r="D26" s="42"/>
+      <c r="E26" s="36"/>
+      <c r="F26" s="36"/>
+      <c r="G26" s="36"/>
+      <c r="H26" s="37"/>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A27" s="27"/>
+      <c r="A27" s="30"/>
       <c r="B27" s="19"/>
       <c r="C27" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="D27" s="36"/>
-      <c r="E27" s="41"/>
-      <c r="F27" s="41"/>
-      <c r="G27" s="41"/>
-      <c r="H27" s="38"/>
+      <c r="D27" s="42"/>
+      <c r="E27" s="36"/>
+      <c r="F27" s="36"/>
+      <c r="G27" s="36"/>
+      <c r="H27" s="37"/>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A28" s="27"/>
+      <c r="A28" s="30"/>
       <c r="B28" s="19"/>
       <c r="C28" s="3"/>
-      <c r="D28" s="36"/>
-      <c r="E28" s="41"/>
-      <c r="F28" s="41"/>
-      <c r="G28" s="41"/>
-      <c r="H28" s="38"/>
+      <c r="D28" s="42"/>
+      <c r="E28" s="36"/>
+      <c r="F28" s="36"/>
+      <c r="G28" s="36"/>
+      <c r="H28" s="37"/>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A29" s="27"/>
+      <c r="A29" s="30"/>
       <c r="B29" s="19"/>
       <c r="C29" s="11" t="s">
         <v>114</v>
       </c>
-      <c r="D29" s="36"/>
-      <c r="E29" s="41"/>
-      <c r="F29" s="41"/>
-      <c r="G29" s="41"/>
-      <c r="H29" s="38"/>
+      <c r="D29" s="42"/>
+      <c r="E29" s="36"/>
+      <c r="F29" s="36"/>
+      <c r="G29" s="36"/>
+      <c r="H29" s="37"/>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A30" s="27"/>
+      <c r="A30" s="30"/>
       <c r="B30" s="19"/>
       <c r="C30" s="12" t="s">
         <v>115</v>
       </c>
-      <c r="D30" s="36"/>
-      <c r="E30" s="41"/>
-      <c r="F30" s="41"/>
-      <c r="G30" s="41"/>
-      <c r="H30" s="38"/>
+      <c r="D30" s="42"/>
+      <c r="E30" s="36"/>
+      <c r="F30" s="36"/>
+      <c r="G30" s="36"/>
+      <c r="H30" s="37"/>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A31" s="27"/>
+      <c r="A31" s="30"/>
       <c r="B31" s="19"/>
       <c r="C31" s="6" t="s">
         <v>116</v>
       </c>
-      <c r="D31" s="36"/>
-      <c r="E31" s="41"/>
-      <c r="F31" s="41"/>
-      <c r="G31" s="41"/>
-      <c r="H31" s="38"/>
+      <c r="D31" s="42"/>
+      <c r="E31" s="36"/>
+      <c r="F31" s="36"/>
+      <c r="G31" s="36"/>
+      <c r="H31" s="37"/>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A32" s="27"/>
+      <c r="A32" s="30"/>
       <c r="B32" s="19"/>
       <c r="C32" s="6" t="s">
         <v>117</v>
       </c>
-      <c r="D32" s="36"/>
-      <c r="E32" s="41"/>
-      <c r="F32" s="41"/>
-      <c r="G32" s="41"/>
-      <c r="H32" s="38"/>
+      <c r="D32" s="42"/>
+      <c r="E32" s="36"/>
+      <c r="F32" s="36"/>
+      <c r="G32" s="36"/>
+      <c r="H32" s="37"/>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A33" s="27"/>
+      <c r="A33" s="30"/>
       <c r="B33" s="19"/>
       <c r="C33" s="12" t="s">
         <v>118</v>
       </c>
-      <c r="D33" s="36"/>
-      <c r="E33" s="41"/>
-      <c r="F33" s="41"/>
-      <c r="G33" s="41"/>
-      <c r="H33" s="38"/>
+      <c r="D33" s="42"/>
+      <c r="E33" s="36"/>
+      <c r="F33" s="36"/>
+      <c r="G33" s="36"/>
+      <c r="H33" s="37"/>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A34" s="27"/>
+      <c r="A34" s="30"/>
       <c r="B34" s="19"/>
       <c r="C34" s="6" t="s">
         <v>119</v>
       </c>
-      <c r="D34" s="36"/>
-      <c r="E34" s="41"/>
-      <c r="F34" s="41"/>
-      <c r="G34" s="41"/>
-      <c r="H34" s="38"/>
+      <c r="D34" s="42"/>
+      <c r="E34" s="36"/>
+      <c r="F34" s="36"/>
+      <c r="G34" s="36"/>
+      <c r="H34" s="37"/>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A35" s="27"/>
+      <c r="A35" s="30"/>
       <c r="B35" s="19"/>
       <c r="C35" s="6" t="s">
         <v>120</v>
       </c>
-      <c r="D35" s="36"/>
-      <c r="E35" s="41"/>
-      <c r="F35" s="41"/>
-      <c r="G35" s="41"/>
-      <c r="H35" s="38"/>
+      <c r="D35" s="42"/>
+      <c r="E35" s="36"/>
+      <c r="F35" s="36"/>
+      <c r="G35" s="36"/>
+      <c r="H35" s="37"/>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A36" s="27"/>
+      <c r="A36" s="30"/>
       <c r="B36" s="19"/>
       <c r="C36" s="12" t="s">
         <v>121</v>
       </c>
-      <c r="D36" s="36"/>
-      <c r="E36" s="41"/>
-      <c r="F36" s="41"/>
-      <c r="G36" s="41"/>
-      <c r="H36" s="38"/>
+      <c r="D36" s="42"/>
+      <c r="E36" s="36"/>
+      <c r="F36" s="36"/>
+      <c r="G36" s="36"/>
+      <c r="H36" s="37"/>
     </row>
     <row r="37" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A37" s="26"/>
+      <c r="A37" s="29"/>
       <c r="B37" s="19"/>
       <c r="C37" s="6" t="s">
         <v>122</v>
       </c>
-      <c r="D37" s="37"/>
-      <c r="E37" s="41"/>
-      <c r="F37" s="41"/>
-      <c r="G37" s="41"/>
-      <c r="H37" s="38"/>
+      <c r="D37" s="41"/>
+      <c r="E37" s="36"/>
+      <c r="F37" s="36"/>
+      <c r="G37" s="36"/>
+      <c r="H37" s="37"/>
     </row>
     <row r="38" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A38" s="14" t="s">
@@ -4644,13 +4650,13 @@
       <c r="D38" s="16" t="s">
         <v>144</v>
       </c>
-      <c r="E38" s="40" t="s">
+      <c r="E38" s="26" t="s">
         <v>170</v>
       </c>
-      <c r="F38" s="40">
+      <c r="F38" s="26">
         <v>5051</v>
       </c>
-      <c r="G38" s="40"/>
+      <c r="G38" s="26"/>
     </row>
     <row r="39" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A39" s="14" t="s">
@@ -4663,9 +4669,9 @@
       <c r="D39" s="16" t="s">
         <v>145</v>
       </c>
-      <c r="E39" s="40"/>
-      <c r="F39" s="40"/>
-      <c r="G39" s="40"/>
+      <c r="E39" s="26"/>
+      <c r="F39" s="26"/>
+      <c r="G39" s="26"/>
     </row>
     <row r="40" spans="1:8" ht="40.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A40" s="14" t="s">
@@ -4678,11 +4684,11 @@
       <c r="D40" s="16" t="s">
         <v>125</v>
       </c>
-      <c r="E40" s="40" t="s">
+      <c r="E40" s="26" t="s">
         <v>175</v>
       </c>
-      <c r="F40" s="40"/>
-      <c r="G40" s="40"/>
+      <c r="F40" s="26"/>
+      <c r="G40" s="26"/>
     </row>
     <row r="41" spans="1:8" ht="30.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A41" s="14" t="s">
@@ -4695,9 +4701,13 @@
       <c r="D41" s="16" t="s">
         <v>125</v>
       </c>
-      <c r="E41" s="40"/>
-      <c r="F41" s="40"/>
-      <c r="G41" s="40"/>
+      <c r="E41" s="26" t="s">
+        <v>170</v>
+      </c>
+      <c r="F41" s="26" t="s">
+        <v>192</v>
+      </c>
+      <c r="G41" s="26"/>
     </row>
     <row r="42" spans="1:8" ht="40.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A42" s="14" t="s">
@@ -4708,9 +4718,13 @@
         <v>130</v>
       </c>
       <c r="D42" s="16"/>
-      <c r="E42" s="40"/>
-      <c r="F42" s="40"/>
-      <c r="G42" s="40"/>
+      <c r="E42" s="26" t="s">
+        <v>170</v>
+      </c>
+      <c r="F42" s="26" t="s">
+        <v>193</v>
+      </c>
+      <c r="G42" s="26"/>
     </row>
     <row r="43" spans="1:8" ht="20.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A43" s="14" t="s">
@@ -4723,50 +4737,56 @@
       <c r="D43" s="16" t="s">
         <v>149</v>
       </c>
-      <c r="E43" s="40"/>
-      <c r="F43" s="40"/>
-      <c r="G43" s="40"/>
+      <c r="E43" s="26" t="s">
+        <v>170</v>
+      </c>
+      <c r="F43" s="26" t="s">
+        <v>193</v>
+      </c>
+      <c r="G43" s="26"/>
     </row>
     <row r="44" spans="1:8" ht="27" x14ac:dyDescent="0.35">
-      <c r="A44" s="25" t="s">
+      <c r="A44" s="28" t="s">
         <v>132</v>
       </c>
       <c r="B44" s="17"/>
       <c r="C44" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="D44" s="35" t="s">
+      <c r="D44" s="40" t="s">
         <v>144</v>
       </c>
-      <c r="E44" s="41"/>
-      <c r="F44" s="41"/>
-      <c r="G44" s="41"/>
-      <c r="H44" s="38"/>
+      <c r="E44" s="36" t="s">
+        <v>170</v>
+      </c>
+      <c r="F44" s="36"/>
+      <c r="G44" s="36"/>
+      <c r="H44" s="37"/>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A45" s="27"/>
+      <c r="A45" s="30"/>
       <c r="B45" s="19"/>
       <c r="C45" s="6" t="e">
         <f>--resources="cpus(prod):8; cpus(stage):2 mem(*):15360; disk(*):710534; ports(*):[31000-32000]"</f>
         <v>#VALUE!</v>
       </c>
-      <c r="D45" s="36"/>
-      <c r="E45" s="41"/>
-      <c r="F45" s="41"/>
-      <c r="G45" s="41"/>
-      <c r="H45" s="38"/>
+      <c r="D45" s="42"/>
+      <c r="E45" s="36"/>
+      <c r="F45" s="36"/>
+      <c r="G45" s="36"/>
+      <c r="H45" s="37"/>
     </row>
     <row r="46" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A46" s="26"/>
+      <c r="A46" s="29"/>
       <c r="B46" s="19"/>
       <c r="C46" s="4" t="s">
         <v>134</v>
       </c>
-      <c r="D46" s="37"/>
-      <c r="E46" s="41"/>
-      <c r="F46" s="41"/>
-      <c r="G46" s="41"/>
-      <c r="H46" s="38"/>
+      <c r="D46" s="41"/>
+      <c r="E46" s="36"/>
+      <c r="F46" s="36"/>
+      <c r="G46" s="36"/>
+      <c r="H46" s="37"/>
     </row>
     <row r="47" spans="1:8" ht="30.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A47" s="14" t="s">
@@ -4779,13 +4799,13 @@
       <c r="D47" s="16" t="s">
         <v>125</v>
       </c>
-      <c r="E47" s="40" t="s">
+      <c r="E47" s="26" t="s">
         <v>175</v>
       </c>
-      <c r="F47" s="42" t="s">
+      <c r="F47" s="27" t="s">
         <v>191</v>
       </c>
-      <c r="G47" s="40"/>
+      <c r="G47" s="26"/>
     </row>
     <row r="48" spans="1:8" ht="20.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A48" s="14" t="s">
@@ -4798,13 +4818,13 @@
       <c r="D48" s="16" t="s">
         <v>144</v>
       </c>
-      <c r="E48" s="40" t="s">
+      <c r="E48" s="26" t="s">
         <v>189</v>
       </c>
-      <c r="F48" s="42" t="s">
+      <c r="F48" s="27" t="s">
         <v>190</v>
       </c>
-      <c r="G48" s="40"/>
+      <c r="G48" s="26"/>
     </row>
     <row r="49" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A49" s="14" t="s">
@@ -4817,13 +4837,13 @@
       <c r="D49" s="16" t="s">
         <v>144</v>
       </c>
-      <c r="E49" s="40" t="s">
+      <c r="E49" s="26" t="s">
         <v>175</v>
       </c>
-      <c r="F49" s="42" t="s">
+      <c r="F49" s="27" t="s">
         <v>188</v>
       </c>
-      <c r="G49" s="40"/>
+      <c r="G49" s="26"/>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A50" s="14" t="s">
@@ -4836,14 +4856,21 @@
       <c r="D50" s="16" t="s">
         <v>144</v>
       </c>
-      <c r="E50" s="40" t="s">
+      <c r="E50" s="26" t="s">
         <v>170</v>
       </c>
-      <c r="F50" s="40"/>
-      <c r="G50" s="40"/>
+      <c r="F50" s="26"/>
+      <c r="G50" s="26"/>
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="A23:A37"/>
+    <mergeCell ref="A44:A46"/>
+    <mergeCell ref="D6:D7"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="D23:D37"/>
+    <mergeCell ref="D44:D46"/>
     <mergeCell ref="E44:E46"/>
     <mergeCell ref="F44:F46"/>
     <mergeCell ref="G44:G46"/>
@@ -4856,13 +4883,6 @@
     <mergeCell ref="F23:F37"/>
     <mergeCell ref="G23:G37"/>
     <mergeCell ref="H23:H37"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="A23:A37"/>
-    <mergeCell ref="A44:A46"/>
-    <mergeCell ref="D6:D7"/>
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="D23:D37"/>
-    <mergeCell ref="D44:D46"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C4" r:id="rId1" location="containerizer" display="https://open.mesosphere.com/reference/glossary/ - containerizer"/>

</xml_diff>

<commit_message>
finish UI type for Master
</commit_message>
<xml_diff>
--- a/configuration flags.xlsx
+++ b/configuration flags.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12840" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12840" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="master-flag" sheetId="1" r:id="rId1"/>
@@ -130,7 +130,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="487" uniqueCount="194">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="517" uniqueCount="199">
   <si>
     <t>Flag</t>
   </si>
@@ -2068,6 +2068,21 @@
   </si>
   <si>
     <t>1 secs</t>
+  </si>
+  <si>
+    <t>10 secs</t>
+  </si>
+  <si>
+    <t>--root_submissions</t>
+  </si>
+  <si>
+    <t>10 mins</t>
+  </si>
+  <si>
+    <t>--no-registry_strict</t>
+  </si>
+  <si>
+    <t>5 secs</t>
   </si>
 </sst>
 </file>
@@ -2231,7 +2246,7 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1" indent="1"/>
@@ -2300,12 +2315,10 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="13" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -2330,12 +2343,6 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2350,6 +2357,33 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="11">
@@ -2809,7 +2843,7 @@
       </c>
     </row>
     <row r="17" spans="1:2" ht="20" x14ac:dyDescent="0.35">
-      <c r="A17" s="28" t="s">
+      <c r="A17" s="26" t="s">
         <v>32</v>
       </c>
       <c r="B17" s="2" t="s">
@@ -2817,7 +2851,7 @@
       </c>
     </row>
     <row r="18" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A18" s="29"/>
+      <c r="A18" s="27"/>
       <c r="B18" s="4" t="s">
         <v>34</v>
       </c>
@@ -2943,7 +2977,7 @@
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A34" s="28" t="s">
+      <c r="A34" s="26" t="s">
         <v>65</v>
       </c>
       <c r="B34" s="2" t="s">
@@ -2951,49 +2985,49 @@
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A35" s="30"/>
+      <c r="A35" s="28"/>
       <c r="B35" s="5" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A36" s="30"/>
+      <c r="A36" s="28"/>
       <c r="B36" s="5" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A37" s="30"/>
+      <c r="A37" s="28"/>
       <c r="B37" s="5" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A38" s="30"/>
+      <c r="A38" s="28"/>
       <c r="B38" s="6" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A39" s="30"/>
+      <c r="A39" s="28"/>
       <c r="B39" s="6" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A40" s="30"/>
+      <c r="A40" s="28"/>
       <c r="B40" s="6" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A41" s="30"/>
+      <c r="A41" s="28"/>
       <c r="B41" s="7" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="42" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A42" s="29"/>
+      <c r="A42" s="27"/>
       <c r="B42" s="8" t="s">
         <v>74</v>
       </c>
@@ -3079,7 +3113,7 @@
       </c>
     </row>
     <row r="6" spans="1:2" ht="20" x14ac:dyDescent="0.35">
-      <c r="A6" s="28" t="s">
+      <c r="A6" s="26" t="s">
         <v>85</v>
       </c>
       <c r="B6" s="2" t="s">
@@ -3087,7 +3121,7 @@
       </c>
     </row>
     <row r="7" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="29"/>
+      <c r="A7" s="27"/>
       <c r="B7" s="6" t="s">
         <v>87</v>
       </c>
@@ -3213,7 +3247,7 @@
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A23" s="28" t="s">
+      <c r="A23" s="26" t="s">
         <v>108</v>
       </c>
       <c r="B23" s="2" t="s">
@@ -3221,83 +3255,83 @@
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A24" s="30"/>
+      <c r="A24" s="28"/>
       <c r="B24" s="5" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A25" s="30"/>
+      <c r="A25" s="28"/>
       <c r="B25" s="5" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A26" s="30"/>
+      <c r="A26" s="28"/>
       <c r="B26" s="5" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A27" s="30"/>
+      <c r="A27" s="28"/>
       <c r="B27" s="4" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A28" s="30"/>
+      <c r="A28" s="28"/>
       <c r="B28" s="3"/>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A29" s="30"/>
+      <c r="A29" s="28"/>
       <c r="B29" s="11" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A30" s="30"/>
+      <c r="A30" s="28"/>
       <c r="B30" s="12" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A31" s="30"/>
+      <c r="A31" s="28"/>
       <c r="B31" s="6" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A32" s="30"/>
+      <c r="A32" s="28"/>
       <c r="B32" s="6" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A33" s="30"/>
+      <c r="A33" s="28"/>
       <c r="B33" s="12" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A34" s="30"/>
+      <c r="A34" s="28"/>
       <c r="B34" s="6" t="s">
         <v>119</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A35" s="30"/>
+      <c r="A35" s="28"/>
       <c r="B35" s="6" t="s">
         <v>120</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A36" s="30"/>
+      <c r="A36" s="28"/>
       <c r="B36" s="12" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A37" s="29"/>
+      <c r="A37" s="27"/>
       <c r="B37" s="6" t="s">
         <v>122</v>
       </c>
@@ -3351,7 +3385,7 @@
       </c>
     </row>
     <row r="44" spans="1:2" ht="27" x14ac:dyDescent="0.35">
-      <c r="A44" s="28" t="s">
+      <c r="A44" s="26" t="s">
         <v>132</v>
       </c>
       <c r="B44" s="2" t="s">
@@ -3359,14 +3393,14 @@
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A45" s="30"/>
+      <c r="A45" s="28"/>
       <c r="B45" s="6" t="e">
         <f>--resources="cpus(prod):8; cpus(stage):2 mem(*):15360; disk(*):710534; ports(*):[31000-32000]"</f>
         <v>#VALUE!</v>
       </c>
     </row>
     <row r="46" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A46" s="29"/>
+      <c r="A46" s="27"/>
       <c r="B46" s="4" t="s">
         <v>134</v>
       </c>
@@ -3428,11 +3462,11 @@
   </sheetPr>
   <dimension ref="A1:I43"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="150" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D9" sqref="D9"/>
+      <selection pane="bottomRight" activeCell="H19" activeCellId="1" sqref="E31:E42 H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3483,12 +3517,15 @@
       <c r="D2" s="16" t="s">
         <v>143</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="40" t="s">
         <v>170</v>
       </c>
-      <c r="F2">
+      <c r="F2" s="40">
         <v>1</v>
       </c>
+      <c r="G2" s="40"/>
+      <c r="H2" s="40"/>
+      <c r="I2" s="25"/>
     </row>
     <row r="3" spans="1:9" ht="40.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="14" t="s">
@@ -3501,12 +3538,15 @@
       <c r="D3" s="16" t="s">
         <v>142</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="40" t="s">
         <v>173</v>
       </c>
-      <c r="F3" s="24" t="s">
+      <c r="F3" s="45" t="s">
         <v>168</v>
       </c>
+      <c r="G3" s="40"/>
+      <c r="H3" s="40"/>
+      <c r="I3" s="25"/>
     </row>
     <row r="4" spans="1:9" ht="50.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A4" s="14" t="s">
@@ -3519,12 +3559,15 @@
       <c r="D4" s="16" t="s">
         <v>142</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="40" t="s">
         <v>173</v>
       </c>
-      <c r="F4" s="24" t="s">
+      <c r="F4" s="45" t="s">
         <v>179</v>
       </c>
+      <c r="G4" s="40"/>
+      <c r="H4" s="40"/>
+      <c r="I4" s="25"/>
     </row>
     <row r="5" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" s="14" t="s">
@@ -3537,9 +3580,13 @@
       <c r="D5" s="16" t="s">
         <v>144</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" s="40" t="s">
         <v>170</v>
       </c>
+      <c r="F5" s="43"/>
+      <c r="G5" s="40"/>
+      <c r="H5" s="40"/>
+      <c r="I5" s="25"/>
     </row>
     <row r="6" spans="1:9" ht="60.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A6" s="14" t="s">
@@ -3552,12 +3599,15 @@
       <c r="D6" s="16" t="s">
         <v>142</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6" s="40" t="s">
         <v>170</v>
       </c>
-      <c r="H6" t="s">
+      <c r="F6" s="43"/>
+      <c r="G6" s="40"/>
+      <c r="H6" s="40" t="s">
         <v>180</v>
       </c>
+      <c r="I6" s="25"/>
     </row>
     <row r="7" spans="1:9" ht="20.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A7" s="14" t="s">
@@ -3570,12 +3620,15 @@
       <c r="D7" s="16" t="s">
         <v>143</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E7" s="40" t="s">
         <v>170</v>
       </c>
-      <c r="F7" t="s">
+      <c r="F7" s="43" t="s">
         <v>181</v>
       </c>
+      <c r="G7" s="40"/>
+      <c r="H7" s="40"/>
+      <c r="I7" s="25"/>
     </row>
     <row r="8" spans="1:9" ht="20.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A8" s="14" t="s">
@@ -3588,12 +3641,15 @@
       <c r="D8" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E8" s="40" t="s">
         <v>173</v>
       </c>
-      <c r="F8" s="24" t="s">
+      <c r="F8" s="45" t="s">
         <v>182</v>
       </c>
+      <c r="G8" s="40"/>
+      <c r="H8" s="40"/>
+      <c r="I8" s="25"/>
     </row>
     <row r="9" spans="1:9" ht="20.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A9" s="14" t="s">
@@ -3606,12 +3662,15 @@
       <c r="D9" s="16" t="s">
         <v>146</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E9" s="40" t="s">
         <v>170</v>
       </c>
-      <c r="F9" s="24" t="s">
+      <c r="F9" s="45" t="s">
         <v>183</v>
       </c>
+      <c r="G9" s="40"/>
+      <c r="H9" s="40"/>
+      <c r="I9" s="25"/>
     </row>
     <row r="10" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A10" s="14" t="s">
@@ -3624,9 +3683,13 @@
       <c r="D10" s="16" t="s">
         <v>144</v>
       </c>
-      <c r="E10" t="s">
+      <c r="E10" s="40" t="s">
         <v>170</v>
       </c>
+      <c r="F10" s="43"/>
+      <c r="G10" s="40"/>
+      <c r="H10" s="40"/>
+      <c r="I10" s="25"/>
     </row>
     <row r="11" spans="1:9" ht="30.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A11" s="14" t="s">
@@ -3639,12 +3702,15 @@
       <c r="D11" s="16" t="s">
         <v>145</v>
       </c>
-      <c r="E11" t="s">
+      <c r="E11" s="40" t="s">
         <v>173</v>
       </c>
-      <c r="F11" s="24" t="s">
+      <c r="F11" s="45" t="s">
         <v>184</v>
       </c>
+      <c r="G11" s="40"/>
+      <c r="H11" s="40"/>
+      <c r="I11" s="25"/>
     </row>
     <row r="12" spans="1:9" ht="20.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A12" s="14" t="s">
@@ -3657,9 +3723,13 @@
       <c r="D12" s="16" t="s">
         <v>145</v>
       </c>
-      <c r="E12" t="s">
+      <c r="E12" s="40" t="s">
         <v>170</v>
       </c>
+      <c r="F12" s="43"/>
+      <c r="G12" s="40"/>
+      <c r="H12" s="40"/>
+      <c r="I12" s="25"/>
     </row>
     <row r="13" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A13" s="14" t="s">
@@ -3672,12 +3742,15 @@
       <c r="D13" s="16" t="s">
         <v>145</v>
       </c>
-      <c r="E13" t="s">
+      <c r="E13" s="40" t="s">
         <v>170</v>
       </c>
-      <c r="F13">
+      <c r="F13" s="43">
         <v>0</v>
       </c>
+      <c r="G13" s="40"/>
+      <c r="H13" s="40"/>
+      <c r="I13" s="25"/>
     </row>
     <row r="14" spans="1:9" ht="20.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A14" s="14" t="s">
@@ -3690,12 +3763,15 @@
       <c r="D14" s="16" t="s">
         <v>145</v>
       </c>
-      <c r="E14" t="s">
+      <c r="E14" s="40" t="s">
         <v>173</v>
       </c>
-      <c r="F14" s="24" t="s">
+      <c r="F14" s="45" t="s">
         <v>185</v>
       </c>
+      <c r="G14" s="40"/>
+      <c r="H14" s="40"/>
+      <c r="I14" s="25"/>
     </row>
     <row r="15" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A15" s="14" t="s">
@@ -3708,12 +3784,15 @@
       <c r="D15" s="16" t="s">
         <v>144</v>
       </c>
-      <c r="E15" t="s">
+      <c r="E15" s="40" t="s">
         <v>170</v>
       </c>
-      <c r="F15">
+      <c r="F15" s="43">
         <v>5051</v>
       </c>
+      <c r="G15" s="40"/>
+      <c r="H15" s="40"/>
+      <c r="I15" s="25"/>
     </row>
     <row r="16" spans="1:9" ht="20.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A16" s="14" t="s">
@@ -3726,26 +3805,45 @@
       <c r="D16" s="16" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" ht="20.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="28" t="s">
+      <c r="E16" s="43" t="s">
+        <v>175</v>
+      </c>
+      <c r="F16" s="43"/>
+      <c r="G16" s="40"/>
+      <c r="H16" s="40"/>
+      <c r="I16" s="25"/>
+    </row>
+    <row r="17" spans="1:9" ht="20.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="26" t="s">
         <v>32</v>
       </c>
       <c r="B17" s="17"/>
-      <c r="C17" s="31" t="s">
+      <c r="C17" s="29" t="s">
         <v>147</v>
       </c>
-      <c r="D17" s="33" t="s">
+      <c r="D17" s="31" t="s">
         <v>146</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A18" s="29"/>
+      <c r="E17" s="44" t="s">
+        <v>170</v>
+      </c>
+      <c r="F17" s="41"/>
+      <c r="G17" s="41"/>
+      <c r="H17" s="41"/>
+      <c r="I17" s="39"/>
+    </row>
+    <row r="18" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A18" s="27"/>
       <c r="B18" s="18"/>
-      <c r="C18" s="32"/>
-      <c r="D18" s="34"/>
-    </row>
-    <row r="19" spans="1:4" ht="77.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C18" s="30"/>
+      <c r="D18" s="32"/>
+      <c r="E18" s="44"/>
+      <c r="F18" s="41"/>
+      <c r="G18" s="41"/>
+      <c r="H18" s="41"/>
+      <c r="I18" s="39"/>
+    </row>
+    <row r="19" spans="1:9" ht="77.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A19" s="14" t="s">
         <v>35</v>
       </c>
@@ -3756,8 +3854,17 @@
       <c r="D19" s="16" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" ht="20.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E19" s="43" t="s">
+        <v>170</v>
+      </c>
+      <c r="F19" s="47">
+        <v>1</v>
+      </c>
+      <c r="G19" s="40"/>
+      <c r="H19" s="40"/>
+      <c r="I19" s="25"/>
+    </row>
+    <row r="20" spans="1:9" ht="20.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A20" s="14" t="s">
         <v>37</v>
       </c>
@@ -3768,8 +3875,17 @@
       <c r="D20" s="16" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" ht="20.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E20" s="40" t="s">
+        <v>170</v>
+      </c>
+      <c r="F20" s="43" t="s">
+        <v>146</v>
+      </c>
+      <c r="G20" s="40"/>
+      <c r="H20" s="40"/>
+      <c r="I20" s="25"/>
+    </row>
+    <row r="21" spans="1:9" ht="20.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A21" s="14" t="s">
         <v>39</v>
       </c>
@@ -3780,8 +3896,17 @@
       <c r="D21" s="16" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" ht="20.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E21" s="40" t="s">
+        <v>170</v>
+      </c>
+      <c r="F21" s="43" t="s">
+        <v>186</v>
+      </c>
+      <c r="G21" s="40"/>
+      <c r="H21" s="40"/>
+      <c r="I21" s="25"/>
+    </row>
+    <row r="22" spans="1:9" ht="20.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A22" s="14" t="s">
         <v>41</v>
       </c>
@@ -3792,8 +3917,17 @@
       <c r="D22" s="16" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" ht="20.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E22" s="40" t="s">
+        <v>170</v>
+      </c>
+      <c r="F22" s="43" t="s">
+        <v>193</v>
+      </c>
+      <c r="G22" s="40"/>
+      <c r="H22" s="40"/>
+      <c r="I22" s="25"/>
+    </row>
+    <row r="23" spans="1:9" ht="20.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A23" s="14" t="s">
         <v>43</v>
       </c>
@@ -3804,8 +3938,17 @@
       <c r="D23" s="16" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" ht="40.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E23" s="40" t="s">
+        <v>170</v>
+      </c>
+      <c r="F23" s="43" t="s">
+        <v>198</v>
+      </c>
+      <c r="G23" s="40"/>
+      <c r="H23" s="40"/>
+      <c r="I23" s="25"/>
+    </row>
+    <row r="24" spans="1:9" ht="40.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A24" s="14" t="s">
         <v>45</v>
       </c>
@@ -3816,8 +3959,17 @@
       <c r="D24" s="16" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" ht="20.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E24" s="40" t="s">
+        <v>175</v>
+      </c>
+      <c r="F24" s="45" t="s">
+        <v>197</v>
+      </c>
+      <c r="G24" s="40"/>
+      <c r="H24" s="40"/>
+      <c r="I24" s="25"/>
+    </row>
+    <row r="25" spans="1:9" ht="20.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A25" s="14" t="s">
         <v>47</v>
       </c>
@@ -3828,8 +3980,15 @@
       <c r="D25" s="16" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" ht="20.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E25" s="40" t="s">
+        <v>170</v>
+      </c>
+      <c r="F25" s="43"/>
+      <c r="G25" s="40"/>
+      <c r="H25" s="40"/>
+      <c r="I25" s="25"/>
+    </row>
+    <row r="26" spans="1:9" ht="20.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A26" s="14" t="s">
         <v>49</v>
       </c>
@@ -3840,8 +3999,17 @@
       <c r="D26" s="16" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" ht="40.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E26" s="40" t="s">
+        <v>175</v>
+      </c>
+      <c r="F26" s="45" t="s">
+        <v>195</v>
+      </c>
+      <c r="G26" s="40"/>
+      <c r="H26" s="40"/>
+      <c r="I26" s="25"/>
+    </row>
+    <row r="27" spans="1:9" ht="40.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A27" s="14" t="s">
         <v>51</v>
       </c>
@@ -3852,8 +4020,17 @@
       <c r="D27" s="16" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" ht="20.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E27" s="40" t="s">
+        <v>170</v>
+      </c>
+      <c r="F27" s="43" t="s">
+        <v>196</v>
+      </c>
+      <c r="G27" s="40"/>
+      <c r="H27" s="40"/>
+      <c r="I27" s="25"/>
+    </row>
+    <row r="28" spans="1:9" ht="20.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A28" s="14" t="s">
         <v>53</v>
       </c>
@@ -3864,32 +4041,57 @@
       <c r="D28" s="16" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E28" s="40" t="s">
+        <v>170</v>
+      </c>
+      <c r="F28" s="43" t="s">
+        <v>181</v>
+      </c>
+      <c r="G28" s="40"/>
+      <c r="H28" s="40"/>
+      <c r="I28" s="25"/>
+    </row>
+    <row r="29" spans="1:9" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A29" s="14" t="s">
         <v>55</v>
       </c>
       <c r="B29" s="17"/>
-      <c r="C29" s="2" t="s">
+      <c r="C29" s="46" t="s">
         <v>56</v>
       </c>
       <c r="D29" s="16" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" ht="20.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E29" s="40" t="s">
+        <v>175</v>
+      </c>
+      <c r="F29" s="45" t="s">
+        <v>188</v>
+      </c>
+      <c r="G29" s="40"/>
+      <c r="H29" s="40"/>
+      <c r="I29" s="25"/>
+    </row>
+    <row r="30" spans="1:9" ht="20.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A30" s="14" t="s">
         <v>57</v>
       </c>
       <c r="B30" s="17"/>
-      <c r="C30" s="2" t="s">
+      <c r="C30" s="46" t="s">
         <v>58</v>
       </c>
       <c r="D30" s="16" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" ht="90.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E30" s="40" t="s">
+        <v>170</v>
+      </c>
+      <c r="F30" s="43"/>
+      <c r="G30" s="40"/>
+      <c r="H30" s="40"/>
+      <c r="I30" s="25"/>
+    </row>
+    <row r="31" spans="1:9" ht="90.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A31" s="14" t="s">
         <v>59</v>
       </c>
@@ -3900,8 +4102,15 @@
       <c r="D31" s="16" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" ht="20.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E31" s="43" t="s">
+        <v>170</v>
+      </c>
+      <c r="F31" s="43"/>
+      <c r="G31" s="40"/>
+      <c r="H31" s="40"/>
+      <c r="I31" s="25"/>
+    </row>
+    <row r="32" spans="1:9" ht="20.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A32" s="14" t="s">
         <v>61</v>
       </c>
@@ -3910,8 +4119,15 @@
         <v>62</v>
       </c>
       <c r="D32" s="16"/>
-    </row>
-    <row r="33" spans="1:4" ht="17.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E32" s="43" t="s">
+        <v>170</v>
+      </c>
+      <c r="F32" s="43"/>
+      <c r="G32" s="40"/>
+      <c r="H32" s="40"/>
+      <c r="I32" s="25"/>
+    </row>
+    <row r="33" spans="1:9" ht="17.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A33" s="14" t="s">
         <v>63</v>
       </c>
@@ -3922,84 +4138,138 @@
       <c r="D33" s="16" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A34" s="28" t="s">
+      <c r="E33" s="43" t="s">
+        <v>170</v>
+      </c>
+      <c r="F33" s="43"/>
+      <c r="G33" s="40"/>
+      <c r="H33" s="40"/>
+      <c r="I33" s="25"/>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A34" s="26" t="s">
         <v>65</v>
       </c>
       <c r="B34" s="17"/>
       <c r="C34" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="D34" s="33" t="s">
+      <c r="D34" s="31" t="s">
         <v>146</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A35" s="30"/>
+      <c r="E34" s="44" t="s">
+        <v>170</v>
+      </c>
+      <c r="F34" s="41"/>
+      <c r="G34" s="41"/>
+      <c r="H34" s="41"/>
+      <c r="I34" s="39"/>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A35" s="28"/>
       <c r="B35" s="19"/>
       <c r="C35" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="D35" s="35"/>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A36" s="30"/>
+      <c r="D35" s="33"/>
+      <c r="E35" s="44"/>
+      <c r="F35" s="41"/>
+      <c r="G35" s="41"/>
+      <c r="H35" s="41"/>
+      <c r="I35" s="39"/>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A36" s="28"/>
       <c r="B36" s="19"/>
       <c r="C36" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="D36" s="35"/>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A37" s="30"/>
+      <c r="D36" s="33"/>
+      <c r="E36" s="44"/>
+      <c r="F36" s="41"/>
+      <c r="G36" s="41"/>
+      <c r="H36" s="41"/>
+      <c r="I36" s="39"/>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A37" s="28"/>
       <c r="B37" s="19"/>
       <c r="C37" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="D37" s="35"/>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A38" s="30"/>
+      <c r="D37" s="33"/>
+      <c r="E37" s="44"/>
+      <c r="F37" s="41"/>
+      <c r="G37" s="41"/>
+      <c r="H37" s="41"/>
+      <c r="I37" s="39"/>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A38" s="28"/>
       <c r="B38" s="19"/>
       <c r="C38" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="D38" s="35"/>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A39" s="30"/>
+      <c r="D38" s="33"/>
+      <c r="E38" s="44"/>
+      <c r="F38" s="41"/>
+      <c r="G38" s="41"/>
+      <c r="H38" s="41"/>
+      <c r="I38" s="39"/>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A39" s="28"/>
       <c r="B39" s="19"/>
       <c r="C39" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="D39" s="35"/>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A40" s="30"/>
+      <c r="D39" s="33"/>
+      <c r="E39" s="44"/>
+      <c r="F39" s="41"/>
+      <c r="G39" s="41"/>
+      <c r="H39" s="41"/>
+      <c r="I39" s="39"/>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A40" s="28"/>
       <c r="B40" s="19"/>
       <c r="C40" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="D40" s="35"/>
-    </row>
-    <row r="41" spans="1:4" ht="20.5" x14ac:dyDescent="0.35">
-      <c r="A41" s="30"/>
+      <c r="D40" s="33"/>
+      <c r="E40" s="44"/>
+      <c r="F40" s="41"/>
+      <c r="G40" s="41"/>
+      <c r="H40" s="41"/>
+      <c r="I40" s="39"/>
+    </row>
+    <row r="41" spans="1:9" ht="20.5" x14ac:dyDescent="0.35">
+      <c r="A41" s="28"/>
       <c r="B41" s="19"/>
       <c r="C41" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="D41" s="35"/>
-    </row>
-    <row r="42" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A42" s="29"/>
+      <c r="D41" s="33"/>
+      <c r="E41" s="44"/>
+      <c r="F41" s="41"/>
+      <c r="G41" s="41"/>
+      <c r="H41" s="41"/>
+      <c r="I41" s="39"/>
+    </row>
+    <row r="42" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A42" s="27"/>
       <c r="B42" s="19"/>
       <c r="C42" s="8" t="s">
         <v>74</v>
       </c>
-      <c r="D42" s="34"/>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="D42" s="32"/>
+      <c r="E42" s="44"/>
+      <c r="F42" s="41"/>
+      <c r="G42" s="41"/>
+      <c r="H42" s="41"/>
+      <c r="I42" s="39"/>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A43" s="14" t="s">
         <v>75</v>
       </c>
@@ -4010,10 +4280,29 @@
       <c r="D43" s="16" t="s">
         <v>146</v>
       </c>
+      <c r="E43" s="40" t="s">
+        <v>170</v>
+      </c>
+      <c r="F43" s="43" t="s">
+        <v>194</v>
+      </c>
+      <c r="G43" s="40"/>
+      <c r="H43" s="40"/>
+      <c r="I43" s="25"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:D43"/>
-  <mergeCells count="5">
+  <mergeCells count="15">
+    <mergeCell ref="E17:E18"/>
+    <mergeCell ref="F17:F18"/>
+    <mergeCell ref="G17:G18"/>
+    <mergeCell ref="H17:H18"/>
+    <mergeCell ref="I17:I18"/>
+    <mergeCell ref="E34:E42"/>
+    <mergeCell ref="F34:F42"/>
+    <mergeCell ref="G34:G42"/>
+    <mergeCell ref="H34:H42"/>
+    <mergeCell ref="I34:I42"/>
     <mergeCell ref="A17:A18"/>
     <mergeCell ref="A34:A42"/>
     <mergeCell ref="C17:C18"/>
@@ -4021,7 +4310,7 @@
     <mergeCell ref="D34:D42"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
@@ -4035,7 +4324,7 @@
           <x14:formula1>
             <xm:f>fileds!$D$2:$D$9</xm:f>
           </x14:formula1>
-          <xm:sqref>E1:E1048576</xm:sqref>
+          <xm:sqref>E43:E1048576 E1:E17 E19:E34</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -4051,13 +4340,13 @@
   <sheetPr>
     <tabColor theme="3" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:H50"/>
+  <dimension ref="A1:I50"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="150" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScaleNormal="100" zoomScalePageLayoutView="150" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B17" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F44" sqref="F44:F46"/>
+      <selection pane="bottomRight" activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4068,7 +4357,7 @@
     <col min="4" max="4" width="8.81640625" style="15"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="13" t="s">
         <v>163</v>
       </c>
@@ -4093,8 +4382,11 @@
       <c r="H1" t="s">
         <v>161</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" ht="20.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I1" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="20.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="14" t="s">
         <v>77</v>
       </c>
@@ -4105,13 +4397,14 @@
       <c r="D2" s="16" t="s">
         <v>150</v>
       </c>
-      <c r="E2" s="26" t="s">
+      <c r="E2" s="40" t="s">
         <v>170</v>
       </c>
-      <c r="F2" s="26"/>
-      <c r="G2" s="26"/>
-    </row>
-    <row r="3" spans="1:8" ht="30.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="F2" s="43"/>
+      <c r="G2" s="40"/>
+      <c r="H2" s="15"/>
+    </row>
+    <row r="3" spans="1:9" ht="30.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="14" t="s">
         <v>79</v>
       </c>
@@ -4122,15 +4415,16 @@
       <c r="D3" s="16" t="s">
         <v>142</v>
       </c>
-      <c r="E3" s="26" t="s">
+      <c r="E3" s="40" t="s">
         <v>175</v>
       </c>
-      <c r="F3" s="26" t="b">
+      <c r="F3" s="43" t="b">
         <v>1</v>
       </c>
-      <c r="G3" s="26"/>
-    </row>
-    <row r="4" spans="1:8" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="G3" s="40"/>
+      <c r="H3" s="15"/>
+    </row>
+    <row r="4" spans="1:9" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A4" s="14" t="s">
         <v>81</v>
       </c>
@@ -4141,13 +4435,14 @@
       <c r="D4" s="16" t="s">
         <v>151</v>
       </c>
-      <c r="E4" s="26" t="s">
+      <c r="E4" s="40" t="s">
         <v>170</v>
       </c>
-      <c r="F4" s="26"/>
-      <c r="G4" s="26"/>
-    </row>
-    <row r="5" spans="1:8" ht="30.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="F4" s="43"/>
+      <c r="G4" s="40"/>
+      <c r="H4" s="15"/>
+    </row>
+    <row r="5" spans="1:9" ht="30.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" s="14" t="s">
         <v>83</v>
       </c>
@@ -4158,41 +4453,42 @@
       <c r="D5" s="16" t="s">
         <v>142</v>
       </c>
-      <c r="E5" s="26" t="s">
+      <c r="E5" s="40" t="s">
         <v>172</v>
       </c>
-      <c r="F5" s="26"/>
-      <c r="G5" s="26"/>
-    </row>
-    <row r="6" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="38" t="s">
+      <c r="F5" s="43"/>
+      <c r="G5" s="40"/>
+      <c r="H5" s="15"/>
+    </row>
+    <row r="6" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="34" t="s">
         <v>85</v>
       </c>
       <c r="B6" s="20"/>
-      <c r="C6" s="31" t="s">
+      <c r="C6" s="29" t="s">
         <v>152</v>
       </c>
-      <c r="D6" s="40" t="s">
+      <c r="D6" s="36" t="s">
         <v>151</v>
       </c>
-      <c r="E6" s="36" t="s">
+      <c r="E6" s="41" t="s">
         <v>170</v>
       </c>
-      <c r="F6" s="36"/>
-      <c r="G6" s="36"/>
-      <c r="H6" s="37"/>
-    </row>
-    <row r="7" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="39"/>
+      <c r="F6" s="44"/>
+      <c r="G6" s="41"/>
+      <c r="H6" s="42"/>
+    </row>
+    <row r="7" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A7" s="35"/>
       <c r="B7" s="21"/>
-      <c r="C7" s="32"/>
-      <c r="D7" s="41"/>
-      <c r="E7" s="36"/>
-      <c r="F7" s="36"/>
-      <c r="G7" s="36"/>
-      <c r="H7" s="37"/>
-    </row>
-    <row r="8" spans="1:8" ht="37.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C7" s="30"/>
+      <c r="D7" s="37"/>
+      <c r="E7" s="41"/>
+      <c r="F7" s="44"/>
+      <c r="G7" s="41"/>
+      <c r="H7" s="42"/>
+    </row>
+    <row r="8" spans="1:9" ht="37.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A8" s="14" t="s">
         <v>88</v>
       </c>
@@ -4200,16 +4496,17 @@
       <c r="C8" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="D8" s="25" t="s">
+      <c r="D8" s="24" t="s">
         <v>143</v>
       </c>
-      <c r="E8" s="26" t="s">
+      <c r="E8" s="40" t="s">
         <v>170</v>
       </c>
-      <c r="F8" s="26"/>
-      <c r="G8" s="26"/>
-    </row>
-    <row r="9" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="F8" s="43"/>
+      <c r="G8" s="40"/>
+      <c r="H8" s="15"/>
+    </row>
+    <row r="9" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A9" s="14" t="s">
         <v>90</v>
       </c>
@@ -4218,15 +4515,16 @@
         <v>91</v>
       </c>
       <c r="D9" s="16"/>
-      <c r="E9" s="26" t="s">
+      <c r="E9" s="40" t="s">
         <v>170</v>
       </c>
-      <c r="F9" s="26" t="s">
+      <c r="F9" s="43" t="s">
         <v>186</v>
       </c>
-      <c r="G9" s="26"/>
-    </row>
-    <row r="10" spans="1:8" ht="20.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="G9" s="40"/>
+      <c r="H9" s="15"/>
+    </row>
+    <row r="10" spans="1:9" ht="20.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A10" s="14" t="s">
         <v>92</v>
       </c>
@@ -4237,13 +4535,14 @@
       <c r="D10" s="16" t="s">
         <v>143</v>
       </c>
-      <c r="E10" s="26" t="s">
+      <c r="E10" s="40" t="s">
         <v>170</v>
       </c>
-      <c r="F10" s="26"/>
-      <c r="G10" s="26"/>
-    </row>
-    <row r="11" spans="1:8" ht="20.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="F10" s="43"/>
+      <c r="G10" s="40"/>
+      <c r="H10" s="15"/>
+    </row>
+    <row r="11" spans="1:9" ht="20.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A11" s="14" t="s">
         <v>94</v>
       </c>
@@ -4254,13 +4553,14 @@
       <c r="D11" s="16" t="s">
         <v>143</v>
       </c>
-      <c r="E11" s="26" t="s">
+      <c r="E11" s="40" t="s">
         <v>170</v>
       </c>
-      <c r="F11" s="26"/>
-      <c r="G11" s="26"/>
-    </row>
-    <row r="12" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="F11" s="43"/>
+      <c r="G11" s="40"/>
+      <c r="H11" s="15"/>
+    </row>
+    <row r="12" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A12" s="14" t="s">
         <v>96</v>
       </c>
@@ -4271,13 +4571,14 @@
       <c r="D12" s="16" t="s">
         <v>143</v>
       </c>
-      <c r="E12" s="26" t="s">
+      <c r="E12" s="40" t="s">
         <v>170</v>
       </c>
-      <c r="F12" s="26"/>
-      <c r="G12" s="26"/>
-    </row>
-    <row r="13" spans="1:8" ht="20.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="F12" s="43"/>
+      <c r="G12" s="40"/>
+      <c r="H12" s="15"/>
+    </row>
+    <row r="13" spans="1:9" ht="20.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A13" s="14" t="s">
         <v>98</v>
       </c>
@@ -4288,15 +4589,16 @@
       <c r="D13" s="16" t="s">
         <v>143</v>
       </c>
-      <c r="E13" s="26" t="s">
+      <c r="E13" s="40" t="s">
         <v>170</v>
       </c>
-      <c r="F13" s="26" t="s">
+      <c r="F13" s="43" t="s">
         <v>187</v>
       </c>
-      <c r="G13" s="26"/>
-    </row>
-    <row r="14" spans="1:8" ht="20.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="G13" s="40"/>
+      <c r="H13" s="15"/>
+    </row>
+    <row r="14" spans="1:9" ht="20.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A14" s="14" t="s">
         <v>100</v>
       </c>
@@ -4307,13 +4609,14 @@
       <c r="D14" s="16" t="s">
         <v>143</v>
       </c>
-      <c r="E14" s="26" t="s">
+      <c r="E14" s="43" t="s">
         <v>170</v>
       </c>
-      <c r="F14" s="26"/>
-      <c r="G14" s="26"/>
-    </row>
-    <row r="15" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="F14" s="43"/>
+      <c r="G14" s="40"/>
+      <c r="H14" s="15"/>
+    </row>
+    <row r="15" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A15" s="14" t="s">
         <v>14</v>
       </c>
@@ -4324,15 +4627,16 @@
       <c r="D15" s="16" t="s">
         <v>144</v>
       </c>
-      <c r="E15" s="26" t="s">
+      <c r="E15" s="43" t="s">
         <v>175</v>
       </c>
-      <c r="F15" s="27" t="s">
+      <c r="F15" s="45" t="s">
         <v>182</v>
       </c>
-      <c r="G15" s="26"/>
-    </row>
-    <row r="16" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="G15" s="40"/>
+      <c r="H15" s="15"/>
+    </row>
+    <row r="16" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A16" s="14" t="s">
         <v>16</v>
       </c>
@@ -4343,11 +4647,12 @@
       <c r="D16" s="22" t="s">
         <v>144</v>
       </c>
-      <c r="E16" s="26" t="s">
+      <c r="E16" s="43" t="s">
         <v>170</v>
       </c>
-      <c r="F16" s="26"/>
-      <c r="G16" s="26"/>
+      <c r="F16" s="43"/>
+      <c r="G16" s="40"/>
+      <c r="H16" s="15"/>
     </row>
     <row r="17" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A17" s="14" t="s">
@@ -4360,11 +4665,12 @@
       <c r="D17" s="16" t="s">
         <v>144</v>
       </c>
-      <c r="E17" s="26" t="s">
+      <c r="E17" s="43" t="s">
         <v>170</v>
       </c>
-      <c r="F17" s="26"/>
-      <c r="G17" s="26"/>
+      <c r="F17" s="43"/>
+      <c r="G17" s="40"/>
+      <c r="H17" s="15"/>
     </row>
     <row r="18" spans="1:8" ht="30.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A18" s="14" t="s">
@@ -4377,11 +4683,12 @@
       <c r="D18" s="16" t="s">
         <v>144</v>
       </c>
-      <c r="E18" s="26" t="s">
+      <c r="E18" s="43" t="s">
         <v>170</v>
       </c>
-      <c r="F18" s="26"/>
-      <c r="G18" s="26"/>
+      <c r="F18" s="43"/>
+      <c r="G18" s="40"/>
+      <c r="H18" s="15"/>
     </row>
     <row r="19" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A19" s="14" t="s">
@@ -4394,11 +4701,12 @@
       <c r="D19" s="16" t="s">
         <v>144</v>
       </c>
-      <c r="E19" s="26" t="s">
+      <c r="E19" s="43" t="s">
         <v>170</v>
       </c>
-      <c r="F19" s="26"/>
-      <c r="G19" s="26"/>
+      <c r="F19" s="43"/>
+      <c r="G19" s="40"/>
+      <c r="H19" s="15"/>
     </row>
     <row r="20" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A20" s="14" t="s">
@@ -4411,11 +4719,12 @@
       <c r="D20" s="16" t="s">
         <v>145</v>
       </c>
-      <c r="E20" s="26" t="s">
+      <c r="E20" s="43" t="s">
         <v>170</v>
       </c>
-      <c r="F20" s="26"/>
-      <c r="G20" s="26"/>
+      <c r="F20" s="43"/>
+      <c r="G20" s="40"/>
+      <c r="H20" s="15"/>
     </row>
     <row r="21" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A21" s="14" t="s">
@@ -4428,13 +4737,14 @@
       <c r="D21" s="16" t="s">
         <v>145</v>
       </c>
-      <c r="E21" s="26" t="s">
+      <c r="E21" s="43" t="s">
         <v>170</v>
       </c>
-      <c r="F21" s="26">
+      <c r="F21" s="43">
         <v>0</v>
       </c>
-      <c r="G21" s="26"/>
+      <c r="G21" s="40"/>
+      <c r="H21" s="15"/>
     </row>
     <row r="22" spans="1:8" ht="17.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A22" s="14" t="s">
@@ -4447,197 +4757,198 @@
       <c r="D22" s="16" t="s">
         <v>145</v>
       </c>
-      <c r="E22" s="26" t="s">
+      <c r="E22" s="43" t="s">
         <v>173</v>
       </c>
-      <c r="F22" s="26" t="s">
+      <c r="F22" s="43" t="s">
         <v>185</v>
       </c>
-      <c r="G22" s="26"/>
+      <c r="G22" s="40"/>
+      <c r="H22" s="15"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A23" s="28" t="s">
+      <c r="A23" s="26" t="s">
         <v>108</v>
       </c>
       <c r="B23" s="17"/>
       <c r="C23" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="D23" s="40" t="s">
+      <c r="D23" s="36" t="s">
         <v>144</v>
       </c>
-      <c r="E23" s="36" t="s">
+      <c r="E23" s="44" t="s">
         <v>170</v>
       </c>
-      <c r="F23" s="36"/>
-      <c r="G23" s="36"/>
-      <c r="H23" s="37"/>
+      <c r="F23" s="44"/>
+      <c r="G23" s="41"/>
+      <c r="H23" s="42"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A24" s="30"/>
+      <c r="A24" s="28"/>
       <c r="B24" s="19"/>
       <c r="C24" s="5" t="s">
         <v>110</v>
       </c>
-      <c r="D24" s="42"/>
-      <c r="E24" s="36"/>
-      <c r="F24" s="36"/>
-      <c r="G24" s="36"/>
-      <c r="H24" s="37"/>
+      <c r="D24" s="38"/>
+      <c r="E24" s="44"/>
+      <c r="F24" s="44"/>
+      <c r="G24" s="41"/>
+      <c r="H24" s="42"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A25" s="30"/>
+      <c r="A25" s="28"/>
       <c r="B25" s="19"/>
       <c r="C25" s="5" t="s">
         <v>111</v>
       </c>
-      <c r="D25" s="42"/>
-      <c r="E25" s="36"/>
-      <c r="F25" s="36"/>
-      <c r="G25" s="36"/>
-      <c r="H25" s="37"/>
+      <c r="D25" s="38"/>
+      <c r="E25" s="44"/>
+      <c r="F25" s="44"/>
+      <c r="G25" s="41"/>
+      <c r="H25" s="42"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A26" s="30"/>
+      <c r="A26" s="28"/>
       <c r="B26" s="19"/>
       <c r="C26" s="5" t="s">
         <v>112</v>
       </c>
-      <c r="D26" s="42"/>
-      <c r="E26" s="36"/>
-      <c r="F26" s="36"/>
-      <c r="G26" s="36"/>
-      <c r="H26" s="37"/>
+      <c r="D26" s="38"/>
+      <c r="E26" s="44"/>
+      <c r="F26" s="44"/>
+      <c r="G26" s="41"/>
+      <c r="H26" s="42"/>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A27" s="30"/>
+      <c r="A27" s="28"/>
       <c r="B27" s="19"/>
       <c r="C27" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="D27" s="42"/>
-      <c r="E27" s="36"/>
-      <c r="F27" s="36"/>
-      <c r="G27" s="36"/>
-      <c r="H27" s="37"/>
+      <c r="D27" s="38"/>
+      <c r="E27" s="44"/>
+      <c r="F27" s="44"/>
+      <c r="G27" s="41"/>
+      <c r="H27" s="42"/>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A28" s="30"/>
+      <c r="A28" s="28"/>
       <c r="B28" s="19"/>
       <c r="C28" s="3"/>
-      <c r="D28" s="42"/>
-      <c r="E28" s="36"/>
-      <c r="F28" s="36"/>
-      <c r="G28" s="36"/>
-      <c r="H28" s="37"/>
+      <c r="D28" s="38"/>
+      <c r="E28" s="44"/>
+      <c r="F28" s="44"/>
+      <c r="G28" s="41"/>
+      <c r="H28" s="42"/>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A29" s="30"/>
+      <c r="A29" s="28"/>
       <c r="B29" s="19"/>
       <c r="C29" s="11" t="s">
         <v>114</v>
       </c>
-      <c r="D29" s="42"/>
-      <c r="E29" s="36"/>
-      <c r="F29" s="36"/>
-      <c r="G29" s="36"/>
-      <c r="H29" s="37"/>
+      <c r="D29" s="38"/>
+      <c r="E29" s="44"/>
+      <c r="F29" s="44"/>
+      <c r="G29" s="41"/>
+      <c r="H29" s="42"/>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A30" s="30"/>
+      <c r="A30" s="28"/>
       <c r="B30" s="19"/>
       <c r="C30" s="12" t="s">
         <v>115</v>
       </c>
-      <c r="D30" s="42"/>
-      <c r="E30" s="36"/>
-      <c r="F30" s="36"/>
-      <c r="G30" s="36"/>
-      <c r="H30" s="37"/>
+      <c r="D30" s="38"/>
+      <c r="E30" s="44"/>
+      <c r="F30" s="44"/>
+      <c r="G30" s="41"/>
+      <c r="H30" s="42"/>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A31" s="30"/>
+      <c r="A31" s="28"/>
       <c r="B31" s="19"/>
       <c r="C31" s="6" t="s">
         <v>116</v>
       </c>
-      <c r="D31" s="42"/>
-      <c r="E31" s="36"/>
-      <c r="F31" s="36"/>
-      <c r="G31" s="36"/>
-      <c r="H31" s="37"/>
+      <c r="D31" s="38"/>
+      <c r="E31" s="44"/>
+      <c r="F31" s="44"/>
+      <c r="G31" s="41"/>
+      <c r="H31" s="42"/>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A32" s="30"/>
+      <c r="A32" s="28"/>
       <c r="B32" s="19"/>
       <c r="C32" s="6" t="s">
         <v>117</v>
       </c>
-      <c r="D32" s="42"/>
-      <c r="E32" s="36"/>
-      <c r="F32" s="36"/>
-      <c r="G32" s="36"/>
-      <c r="H32" s="37"/>
+      <c r="D32" s="38"/>
+      <c r="E32" s="44"/>
+      <c r="F32" s="44"/>
+      <c r="G32" s="41"/>
+      <c r="H32" s="42"/>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A33" s="30"/>
+      <c r="A33" s="28"/>
       <c r="B33" s="19"/>
       <c r="C33" s="12" t="s">
         <v>118</v>
       </c>
-      <c r="D33" s="42"/>
-      <c r="E33" s="36"/>
-      <c r="F33" s="36"/>
-      <c r="G33" s="36"/>
-      <c r="H33" s="37"/>
+      <c r="D33" s="38"/>
+      <c r="E33" s="44"/>
+      <c r="F33" s="44"/>
+      <c r="G33" s="41"/>
+      <c r="H33" s="42"/>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A34" s="30"/>
+      <c r="A34" s="28"/>
       <c r="B34" s="19"/>
       <c r="C34" s="6" t="s">
         <v>119</v>
       </c>
-      <c r="D34" s="42"/>
-      <c r="E34" s="36"/>
-      <c r="F34" s="36"/>
-      <c r="G34" s="36"/>
-      <c r="H34" s="37"/>
+      <c r="D34" s="38"/>
+      <c r="E34" s="44"/>
+      <c r="F34" s="44"/>
+      <c r="G34" s="41"/>
+      <c r="H34" s="42"/>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A35" s="30"/>
+      <c r="A35" s="28"/>
       <c r="B35" s="19"/>
       <c r="C35" s="6" t="s">
         <v>120</v>
       </c>
-      <c r="D35" s="42"/>
-      <c r="E35" s="36"/>
-      <c r="F35" s="36"/>
-      <c r="G35" s="36"/>
-      <c r="H35" s="37"/>
+      <c r="D35" s="38"/>
+      <c r="E35" s="44"/>
+      <c r="F35" s="44"/>
+      <c r="G35" s="41"/>
+      <c r="H35" s="42"/>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A36" s="30"/>
+      <c r="A36" s="28"/>
       <c r="B36" s="19"/>
       <c r="C36" s="12" t="s">
         <v>121</v>
       </c>
-      <c r="D36" s="42"/>
-      <c r="E36" s="36"/>
-      <c r="F36" s="36"/>
-      <c r="G36" s="36"/>
-      <c r="H36" s="37"/>
+      <c r="D36" s="38"/>
+      <c r="E36" s="44"/>
+      <c r="F36" s="44"/>
+      <c r="G36" s="41"/>
+      <c r="H36" s="42"/>
     </row>
     <row r="37" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A37" s="29"/>
+      <c r="A37" s="27"/>
       <c r="B37" s="19"/>
       <c r="C37" s="6" t="s">
         <v>122</v>
       </c>
-      <c r="D37" s="41"/>
-      <c r="E37" s="36"/>
-      <c r="F37" s="36"/>
-      <c r="G37" s="36"/>
-      <c r="H37" s="37"/>
+      <c r="D37" s="37"/>
+      <c r="E37" s="44"/>
+      <c r="F37" s="44"/>
+      <c r="G37" s="41"/>
+      <c r="H37" s="42"/>
     </row>
     <row r="38" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A38" s="14" t="s">
@@ -4650,13 +4961,14 @@
       <c r="D38" s="16" t="s">
         <v>144</v>
       </c>
-      <c r="E38" s="26" t="s">
+      <c r="E38" s="43" t="s">
         <v>170</v>
       </c>
-      <c r="F38" s="26">
+      <c r="F38" s="43">
         <v>5051</v>
       </c>
-      <c r="G38" s="26"/>
+      <c r="G38" s="40"/>
+      <c r="H38" s="15"/>
     </row>
     <row r="39" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A39" s="14" t="s">
@@ -4669,9 +4981,10 @@
       <c r="D39" s="16" t="s">
         <v>145</v>
       </c>
-      <c r="E39" s="26"/>
-      <c r="F39" s="26"/>
-      <c r="G39" s="26"/>
+      <c r="E39" s="43"/>
+      <c r="F39" s="43"/>
+      <c r="G39" s="40"/>
+      <c r="H39" s="15"/>
     </row>
     <row r="40" spans="1:8" ht="40.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A40" s="14" t="s">
@@ -4684,11 +4997,12 @@
       <c r="D40" s="16" t="s">
         <v>125</v>
       </c>
-      <c r="E40" s="26" t="s">
+      <c r="E40" s="43" t="s">
         <v>175</v>
       </c>
-      <c r="F40" s="26"/>
-      <c r="G40" s="26"/>
+      <c r="F40" s="43"/>
+      <c r="G40" s="40"/>
+      <c r="H40" s="15"/>
     </row>
     <row r="41" spans="1:8" ht="30.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A41" s="14" t="s">
@@ -4701,15 +5015,16 @@
       <c r="D41" s="16" t="s">
         <v>125</v>
       </c>
-      <c r="E41" s="26" t="s">
+      <c r="E41" s="43" t="s">
         <v>170</v>
       </c>
-      <c r="F41" s="26" t="s">
+      <c r="F41" s="43" t="s">
         <v>192</v>
       </c>
-      <c r="G41" s="26"/>
-    </row>
-    <row r="42" spans="1:8" ht="40.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="G41" s="40"/>
+      <c r="H41" s="15"/>
+    </row>
+    <row r="42" spans="1:8" ht="30.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A42" s="14" t="s">
         <v>129</v>
       </c>
@@ -4718,13 +5033,14 @@
         <v>130</v>
       </c>
       <c r="D42" s="16"/>
-      <c r="E42" s="26" t="s">
+      <c r="E42" s="43" t="s">
         <v>170</v>
       </c>
-      <c r="F42" s="26" t="s">
+      <c r="F42" s="43" t="s">
         <v>193</v>
       </c>
-      <c r="G42" s="26"/>
+      <c r="G42" s="40"/>
+      <c r="H42" s="15"/>
     </row>
     <row r="43" spans="1:8" ht="20.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A43" s="14" t="s">
@@ -4737,56 +5053,57 @@
       <c r="D43" s="16" t="s">
         <v>149</v>
       </c>
-      <c r="E43" s="26" t="s">
+      <c r="E43" s="43" t="s">
         <v>170</v>
       </c>
-      <c r="F43" s="26" t="s">
+      <c r="F43" s="43" t="s">
         <v>193</v>
       </c>
-      <c r="G43" s="26"/>
+      <c r="G43" s="40"/>
+      <c r="H43" s="15"/>
     </row>
     <row r="44" spans="1:8" ht="27" x14ac:dyDescent="0.35">
-      <c r="A44" s="28" t="s">
+      <c r="A44" s="26" t="s">
         <v>132</v>
       </c>
       <c r="B44" s="17"/>
       <c r="C44" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="D44" s="40" t="s">
+      <c r="D44" s="36" t="s">
         <v>144</v>
       </c>
-      <c r="E44" s="36" t="s">
+      <c r="E44" s="44" t="s">
         <v>170</v>
       </c>
-      <c r="F44" s="36"/>
-      <c r="G44" s="36"/>
-      <c r="H44" s="37"/>
+      <c r="F44" s="44"/>
+      <c r="G44" s="41"/>
+      <c r="H44" s="42"/>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A45" s="30"/>
+      <c r="A45" s="28"/>
       <c r="B45" s="19"/>
       <c r="C45" s="6" t="e">
         <f>--resources="cpus(prod):8; cpus(stage):2 mem(*):15360; disk(*):710534; ports(*):[31000-32000]"</f>
         <v>#VALUE!</v>
       </c>
-      <c r="D45" s="42"/>
-      <c r="E45" s="36"/>
-      <c r="F45" s="36"/>
-      <c r="G45" s="36"/>
-      <c r="H45" s="37"/>
+      <c r="D45" s="38"/>
+      <c r="E45" s="44"/>
+      <c r="F45" s="44"/>
+      <c r="G45" s="41"/>
+      <c r="H45" s="42"/>
     </row>
     <row r="46" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A46" s="29"/>
+      <c r="A46" s="27"/>
       <c r="B46" s="19"/>
       <c r="C46" s="4" t="s">
         <v>134</v>
       </c>
-      <c r="D46" s="41"/>
-      <c r="E46" s="36"/>
-      <c r="F46" s="36"/>
-      <c r="G46" s="36"/>
-      <c r="H46" s="37"/>
+      <c r="D46" s="37"/>
+      <c r="E46" s="44"/>
+      <c r="F46" s="44"/>
+      <c r="G46" s="41"/>
+      <c r="H46" s="42"/>
     </row>
     <row r="47" spans="1:8" ht="30.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A47" s="14" t="s">
@@ -4799,13 +5116,14 @@
       <c r="D47" s="16" t="s">
         <v>125</v>
       </c>
-      <c r="E47" s="26" t="s">
+      <c r="E47" s="43" t="s">
         <v>175</v>
       </c>
-      <c r="F47" s="27" t="s">
+      <c r="F47" s="45" t="s">
         <v>191</v>
       </c>
-      <c r="G47" s="26"/>
+      <c r="G47" s="40"/>
+      <c r="H47" s="15"/>
     </row>
     <row r="48" spans="1:8" ht="20.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A48" s="14" t="s">
@@ -4818,15 +5136,16 @@
       <c r="D48" s="16" t="s">
         <v>144</v>
       </c>
-      <c r="E48" s="26" t="s">
+      <c r="E48" s="43" t="s">
         <v>189</v>
       </c>
-      <c r="F48" s="27" t="s">
+      <c r="F48" s="45" t="s">
         <v>190</v>
       </c>
-      <c r="G48" s="26"/>
-    </row>
-    <row r="49" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="G48" s="40"/>
+      <c r="H48" s="15"/>
+    </row>
+    <row r="49" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A49" s="14" t="s">
         <v>55</v>
       </c>
@@ -4837,15 +5156,16 @@
       <c r="D49" s="16" t="s">
         <v>144</v>
       </c>
-      <c r="E49" s="26" t="s">
+      <c r="E49" s="43" t="s">
         <v>175</v>
       </c>
-      <c r="F49" s="27" t="s">
+      <c r="F49" s="45" t="s">
         <v>188</v>
       </c>
-      <c r="G49" s="26"/>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="G49" s="40"/>
+      <c r="H49" s="15"/>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A50" s="14" t="s">
         <v>63</v>
       </c>
@@ -4856,21 +5176,15 @@
       <c r="D50" s="16" t="s">
         <v>144</v>
       </c>
-      <c r="E50" s="26" t="s">
+      <c r="E50" s="43" t="s">
         <v>170</v>
       </c>
-      <c r="F50" s="26"/>
-      <c r="G50" s="26"/>
+      <c r="F50" s="40"/>
+      <c r="G50" s="40"/>
+      <c r="H50" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="A23:A37"/>
-    <mergeCell ref="A44:A46"/>
-    <mergeCell ref="D6:D7"/>
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="D23:D37"/>
-    <mergeCell ref="D44:D46"/>
     <mergeCell ref="E44:E46"/>
     <mergeCell ref="F44:F46"/>
     <mergeCell ref="G44:G46"/>
@@ -4883,6 +5197,13 @@
     <mergeCell ref="F23:F37"/>
     <mergeCell ref="G23:G37"/>
     <mergeCell ref="H23:H37"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="A23:A37"/>
+    <mergeCell ref="A44:A46"/>
+    <mergeCell ref="D6:D7"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="D23:D37"/>
+    <mergeCell ref="D44:D46"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C4" r:id="rId1" location="containerizer" display="https://open.mesosphere.com/reference/glossary/ - containerizer"/>

</xml_diff>